<commit_message>
the rest of the edits
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar.xlsx
+++ b/CS320-Spring2024Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB8DC12-63A0-4F83-9712-8DB25A10A286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA119ED1-1776-4C33-A3E8-91FBF0A5E0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="18285" windowHeight="15427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Monday</t>
   </si>
@@ -240,12 +240,6 @@
   </si>
   <si>
     <t>May/Apr</t>
-  </si>
-  <si>
-    <t>Lab 2a: Web
-Applications
-due Noon
-(Marmoset)</t>
   </si>
   <si>
     <t>Intro to Relational Databases, SQL, JDBC, ORM Labs</t>
@@ -568,6 +562,12 @@
 due before class
 (Marmoset)</t>
     </r>
+  </si>
+  <si>
+    <t>Lab 2a: Web
+Applications
+due Noon (after sign-off)
+(Marmoset)</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1622,9 +1622,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1722,6 +1719,15 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2033,8 +2039,8 @@
   </sheetPr>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2056,17 +2062,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="146" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="148"/>
+      <c r="A1" s="145" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="147"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2096,10 +2102,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="138">
+      <c r="A3" s="137">
         <v>15</v>
       </c>
-      <c r="B3" s="133" t="s">
+      <c r="B3" s="132" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="69">
@@ -2131,8 +2137,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="142"/>
-      <c r="B4" s="150"/>
+      <c r="A4" s="141"/>
+      <c r="B4" s="149"/>
       <c r="C4" s="71" t="s">
         <v>7</v>
       </c>
@@ -2153,16 +2159,16 @@
       </c>
       <c r="G4" s="38"/>
       <c r="H4" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" s="41"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="142">
+      <c r="A5" s="141">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="134" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="7">
@@ -2194,17 +2200,17 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="137.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="139"/>
-      <c r="B6" s="134"/>
-      <c r="C6" s="128" t="s">
-        <v>71</v>
+      <c r="A6" s="138"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="127" t="s">
+        <v>70</v>
       </c>
       <c r="D6" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="59"/>
+      <c r="F6" s="150" t="s">
         <v>75</v>
-      </c>
-      <c r="E6" s="59"/>
-      <c r="F6" s="151" t="s">
-        <v>76</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="12" t="s">
@@ -2213,11 +2219,11 @@
       <c r="I6" s="110"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="143">
+      <c r="A7" s="142">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="39">
@@ -2250,10 +2256,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="87.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="136"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="135"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="48" t="s">
         <v>32</v>
@@ -2267,15 +2273,15 @@
         <v>31</v>
       </c>
       <c r="I8" s="111" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="136">
+      <c r="A9" s="135">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="132"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2304,22 +2310,22 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L9" s="122"/>
-      <c r="M9" s="122"/>
-      <c r="N9" s="122"/>
-      <c r="O9" s="122"/>
-      <c r="P9" s="122"/>
-      <c r="Q9" s="122"/>
-      <c r="R9" s="122"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="121"/>
+      <c r="R9" s="121"/>
     </row>
     <row r="10" spans="1:18" ht="80.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="136"/>
-      <c r="B10" s="132"/>
+      <c r="A10" s="135"/>
+      <c r="B10" s="131"/>
       <c r="C10" s="112" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="10" t="s">
@@ -2327,23 +2333,23 @@
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I10" s="13"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="122"/>
-      <c r="N10" s="123"/>
-      <c r="O10" s="122"/>
-      <c r="P10" s="123"/>
-      <c r="Q10" s="122"/>
-      <c r="R10" s="123"/>
+      <c r="M10" s="121"/>
+      <c r="N10" s="122"/>
+      <c r="O10" s="121"/>
+      <c r="P10" s="122"/>
+      <c r="Q10" s="121"/>
+      <c r="R10" s="122"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="136">
+      <c r="A11" s="135">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="132"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2372,24 +2378,24 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="L11" s="122"/>
-      <c r="M11" s="122"/>
-      <c r="N11" s="122"/>
-      <c r="O11" s="122"/>
-      <c r="P11" s="122"/>
-      <c r="Q11" s="122"/>
-      <c r="R11" s="122"/>
+      <c r="L11" s="121"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="121"/>
+      <c r="O11" s="121"/>
+      <c r="P11" s="121"/>
+      <c r="Q11" s="121"/>
+      <c r="R11" s="121"/>
     </row>
     <row r="12" spans="1:18" ht="90.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="136"/>
-      <c r="B12" s="132"/>
-      <c r="C12" s="31" t="s">
-        <v>45</v>
-      </c>
+      <c r="A12" s="135"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="152"/>
       <c r="D12" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="45"/>
+      <c r="E12" s="151" t="s">
+        <v>76</v>
+      </c>
       <c r="F12" s="45" t="s">
         <v>39</v>
       </c>
@@ -2399,19 +2405,19 @@
       </c>
       <c r="I12" s="80"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="122"/>
-      <c r="N12" s="122"/>
-      <c r="O12" s="122"/>
-      <c r="P12" s="123"/>
-      <c r="Q12" s="122"/>
-      <c r="R12" s="123"/>
+      <c r="M12" s="121"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="121"/>
+      <c r="P12" s="122"/>
+      <c r="Q12" s="121"/>
+      <c r="R12" s="122"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="136">
+      <c r="A13" s="135">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="129" t="s">
+      <c r="B13" s="128" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="17">
@@ -2441,24 +2447,24 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L13" s="122"/>
-      <c r="M13" s="122"/>
-      <c r="N13" s="122"/>
-      <c r="O13" s="122"/>
-      <c r="P13" s="122"/>
-      <c r="Q13" s="122"/>
-      <c r="R13" s="124"/>
+      <c r="L13" s="121"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="121"/>
+      <c r="O13" s="121"/>
+      <c r="P13" s="121"/>
+      <c r="Q13" s="121"/>
+      <c r="R13" s="123"/>
     </row>
     <row r="14" spans="1:18" ht="108.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="137"/>
-      <c r="B14" s="130"/>
+      <c r="A14" s="136"/>
+      <c r="B14" s="129"/>
       <c r="C14" s="29"/>
       <c r="D14" s="113" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="93"/>
       <c r="F14" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" s="92" t="s">
         <v>42</v>
@@ -2469,20 +2475,20 @@
       <c r="I14" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="L14" s="124"/>
+      <c r="L14" s="123"/>
       <c r="M14" s="25"/>
-      <c r="N14" s="125"/>
-      <c r="O14" s="122"/>
-      <c r="P14" s="124"/>
-      <c r="Q14" s="122"/>
-      <c r="R14" s="124"/>
+      <c r="N14" s="124"/>
+      <c r="O14" s="121"/>
+      <c r="P14" s="123"/>
+      <c r="Q14" s="121"/>
+      <c r="R14" s="123"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="138">
+      <c r="A15" s="137">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="135" t="s">
+      <c r="B15" s="134" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="69">
@@ -2515,23 +2521,23 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="139"/>
-      <c r="B16" s="134"/>
+      <c r="A16" s="138"/>
+      <c r="B16" s="133"/>
       <c r="C16" s="89" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16" s="96"/>
       <c r="H16" s="66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" s="97"/>
     </row>
@@ -2568,42 +2574,42 @@
       </c>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="1:18" s="127" customFormat="1" ht="21.4" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="126"/>
+    <row r="20" spans="1:18" s="126" customFormat="1" ht="21.4" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="125"/>
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
-      <c r="D20" s="124"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="124"/>
-      <c r="H20" s="124"/>
-      <c r="I20" s="124"/>
-    </row>
-    <row r="21" spans="1:18" s="127" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="126"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="123"/>
+      <c r="G20" s="123"/>
+      <c r="H20" s="123"/>
+      <c r="I20" s="123"/>
+    </row>
+    <row r="21" spans="1:18" s="126" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="125"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="124"/>
-      <c r="F21" s="124"/>
-      <c r="G21" s="124"/>
-      <c r="H21" s="124"/>
-      <c r="I21" s="124"/>
+      <c r="D21" s="123"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="123"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="123"/>
+      <c r="I21" s="123"/>
     </row>
     <row r="22" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="146" t="str">
+      <c r="A22" s="145" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
 (as of 1-24-2024, subject to change)</v>
       </c>
-      <c r="B22" s="147"/>
-      <c r="C22" s="147"/>
-      <c r="D22" s="147"/>
-      <c r="E22" s="147"/>
-      <c r="F22" s="147"/>
-      <c r="G22" s="147"/>
-      <c r="H22" s="147"/>
-      <c r="I22" s="148"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="146"/>
+      <c r="I22" s="147"/>
     </row>
     <row r="23" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="str">
@@ -2641,11 +2647,11 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="149">
+      <c r="A24" s="148">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B24" s="135" t="s">
+      <c r="B24" s="134" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="98">
@@ -2676,24 +2682,24 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="L24" s="124"/>
-      <c r="M24" s="122"/>
-      <c r="N24" s="122"/>
-      <c r="O24" s="122"/>
-      <c r="P24" s="122"/>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="122"/>
+      <c r="L24" s="123"/>
+      <c r="M24" s="121"/>
+      <c r="N24" s="121"/>
+      <c r="O24" s="121"/>
+      <c r="P24" s="121"/>
+      <c r="Q24" s="121"/>
+      <c r="R24" s="121"/>
     </row>
     <row r="25" spans="1:18" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="142"/>
-      <c r="B25" s="135"/>
+      <c r="A25" s="141"/>
+      <c r="B25" s="134"/>
       <c r="C25" s="53"/>
       <c r="D25" s="22" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6" t="s">
@@ -2701,19 +2707,19 @@
       </c>
       <c r="I25" s="36"/>
       <c r="L25" s="25"/>
-      <c r="M25" s="122"/>
-      <c r="N25" s="122"/>
-      <c r="O25" s="122"/>
-      <c r="P25" s="122"/>
-      <c r="Q25" s="122"/>
+      <c r="M25" s="121"/>
+      <c r="N25" s="121"/>
+      <c r="O25" s="121"/>
+      <c r="P25" s="121"/>
+      <c r="Q25" s="121"/>
       <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="142">
+      <c r="A26" s="141">
         <f>A24 - 1</f>
         <v>7</v>
       </c>
-      <c r="B26" s="135"/>
+      <c r="B26" s="134"/>
       <c r="C26" s="7">
         <f>I24 + 1</f>
         <v>17</v>
@@ -2742,50 +2748,50 @@
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="L26" s="122"/>
-      <c r="M26" s="122"/>
-      <c r="N26" s="122"/>
-      <c r="O26" s="122"/>
-      <c r="P26" s="122"/>
-      <c r="Q26" s="122"/>
-      <c r="R26" s="122"/>
+      <c r="L26" s="121"/>
+      <c r="M26" s="121"/>
+      <c r="N26" s="121"/>
+      <c r="O26" s="121"/>
+      <c r="P26" s="121"/>
+      <c r="Q26" s="121"/>
+      <c r="R26" s="121"/>
     </row>
     <row r="27" spans="1:18" ht="129.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="142"/>
-      <c r="B27" s="135"/>
-      <c r="C27" s="121"/>
+      <c r="A27" s="141"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="120"/>
       <c r="D27" s="26" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="114" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F27" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" s="114" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="I27" s="120" t="s">
-        <v>53</v>
-      </c>
       <c r="L27" s="25"/>
-      <c r="M27" s="122"/>
-      <c r="N27" s="124"/>
-      <c r="O27" s="122"/>
-      <c r="P27" s="124"/>
-      <c r="Q27" s="122"/>
+      <c r="M27" s="121"/>
+      <c r="N27" s="123"/>
+      <c r="O27" s="121"/>
+      <c r="P27" s="123"/>
+      <c r="Q27" s="121"/>
       <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="142">
+      <c r="A28" s="141">
         <f>A26 - 1</f>
         <v>6</v>
       </c>
-      <c r="B28" s="135"/>
+      <c r="B28" s="134"/>
       <c r="C28" s="7">
         <f>I26 + 1</f>
         <v>24</v>
@@ -2814,48 +2820,48 @@
         <f t="shared" ref="I28" si="9">H28 + 1</f>
         <v>30</v>
       </c>
-      <c r="L28" s="122"/>
-      <c r="M28" s="122"/>
-      <c r="N28" s="122"/>
-      <c r="O28" s="122"/>
-      <c r="P28" s="122"/>
-      <c r="Q28" s="122"/>
-      <c r="R28" s="122"/>
+      <c r="L28" s="121"/>
+      <c r="M28" s="121"/>
+      <c r="N28" s="121"/>
+      <c r="O28" s="121"/>
+      <c r="P28" s="121"/>
+      <c r="Q28" s="121"/>
+      <c r="R28" s="121"/>
     </row>
     <row r="29" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="139"/>
-      <c r="B29" s="134"/>
+      <c r="A29" s="138"/>
+      <c r="B29" s="133"/>
       <c r="C29" s="115"/>
       <c r="D29" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G29" s="99"/>
       <c r="H29" s="74" t="s">
-        <v>48</v>
-      </c>
-      <c r="I29" s="119" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="I29" s="118" t="s">
+        <v>47</v>
       </c>
       <c r="L29" s="25"/>
-      <c r="M29" s="122"/>
+      <c r="M29" s="121"/>
       <c r="N29" s="25"/>
-      <c r="O29" s="122"/>
+      <c r="O29" s="121"/>
       <c r="P29" s="25"/>
-      <c r="Q29" s="124"/>
+      <c r="Q29" s="123"/>
       <c r="R29" s="25"/>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="143">
+      <c r="A30" s="142">
         <f>A28 -1</f>
         <v>5</v>
       </c>
-      <c r="B30" s="131" t="s">
+      <c r="B30" s="130" t="s">
         <v>43</v>
       </c>
       <c r="C30" s="105">
@@ -2887,30 +2893,32 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="144"/>
-      <c r="B31" s="130"/>
-      <c r="C31" s="118" t="s">
-        <v>66</v>
+      <c r="A31" s="143"/>
+      <c r="B31" s="129"/>
+      <c r="C31" s="153" t="s">
+        <v>47</v>
       </c>
       <c r="D31" s="107" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="27"/>
+        <v>47</v>
+      </c>
+      <c r="E31" s="52" t="s">
+        <v>65</v>
+      </c>
       <c r="F31" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G31" s="81"/>
       <c r="H31" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I31" s="28"/>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="145">
+      <c r="A32" s="144">
         <f>A30 -1</f>
         <v>4</v>
       </c>
-      <c r="B32" s="131" t="s">
+      <c r="B32" s="130" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="62">
@@ -2943,30 +2951,30 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="136"/>
-      <c r="B33" s="132"/>
+      <c r="A33" s="135"/>
+      <c r="B33" s="131"/>
       <c r="C33" s="29"/>
       <c r="D33" s="116" t="s">
         <v>28</v>
       </c>
       <c r="E33" s="117" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G33" s="27"/>
       <c r="H33" s="109" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="136">
+      <c r="A34" s="135">
         <f>A32 -1</f>
         <v>3</v>
       </c>
-      <c r="B34" s="132"/>
+      <c r="B34" s="131"/>
       <c r="C34" s="27">
         <f>I32 + 1</f>
         <v>14</v>
@@ -2997,8 +3005,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="136"/>
-      <c r="B35" s="132"/>
+      <c r="A35" s="135"/>
+      <c r="B35" s="131"/>
       <c r="C35" s="29"/>
       <c r="D35" s="108" t="s">
         <v>6</v>
@@ -3014,11 +3022,11 @@
       <c r="I35" s="28"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="136">
+      <c r="A36" s="135">
         <f>A34 -1</f>
         <v>2</v>
       </c>
-      <c r="B36" s="132"/>
+      <c r="B36" s="131"/>
       <c r="C36" s="29">
         <f>I34 + 1</f>
         <v>21</v>
@@ -3049,8 +3057,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="137"/>
-      <c r="B37" s="130"/>
+      <c r="A37" s="136"/>
+      <c r="B37" s="129"/>
       <c r="C37" s="60"/>
       <c r="D37" s="44" t="s">
         <v>25</v>
@@ -3066,11 +3074,11 @@
       <c r="I37" s="42"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="138">
+      <c r="A38" s="137">
         <f>A36 -1</f>
         <v>1</v>
       </c>
-      <c r="B38" s="133" t="s">
+      <c r="B38" s="132" t="s">
         <v>44</v>
       </c>
       <c r="C38" s="17">
@@ -3102,8 +3110,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="139"/>
-      <c r="B39" s="134"/>
+      <c r="A39" s="138"/>
+      <c r="B39" s="133"/>
       <c r="C39" s="102"/>
       <c r="D39" s="50" t="s">
         <v>6</v>
@@ -3117,14 +3125,14 @@
         <v>38</v>
       </c>
       <c r="I39" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="140" t="s">
+      <c r="A40" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="135" t="s">
+      <c r="B40" s="134" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="20">
@@ -3157,17 +3165,17 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="141"/>
-      <c r="B41" s="134"/>
+      <c r="A41" s="140"/>
+      <c r="B41" s="133"/>
       <c r="C41" s="63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E41" s="64"/>
       <c r="F41" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G41" s="21"/>
       <c r="H41" s="78"/>

</xml_diff>

<commit_message>
updating schedule for Web Apps and development process
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar.xlsx
+++ b/CS320-Spring2024Calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3882A686-D6A5-497C-B59A-B0F066E8395C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDA5D73-739F-4A07-BB49-1C294C01AFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="0" windowWidth="22433" windowHeight="14857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="203" windowWidth="23520" windowHeight="14572" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp24" sheetId="1" r:id="rId1"/>
@@ -136,44 +136,6 @@
 Web Applications Labs Review</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Lecture 4: Web Applications
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Git Lab: Part I
-due
-(in class)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Web
-Applications I
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 2a: Web Applications
-(assigned)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -235,10 +197,6 @@
   <si>
     <t>A02: Individual Project Proposal due Noon
 (Marmoset)</t>
-  </si>
-  <si>
-    <t>A01: Team Project Proposal due Noon
-(Google Doc)</t>
   </si>
   <si>
     <t>Lab 4: SQL
@@ -534,8 +492,26 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Project Introductions
-Lecture 12: Version Control
+      <t xml:space="preserve">Lecture 4: Web Applications
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 2a: Web Applications
+(assigned)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Project Intros
+Lecture 12: Version Control I
 (Git)
 </t>
     </r>
@@ -575,6 +551,30 @@
       <t>Lab 0: ChatGPT
 due 7:00am
 (Marmoset)</t>
+    </r>
+  </si>
+  <si>
+    <t>A01: Team Project Proposal due Noon
+(Marmoset)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Review ChatPT and HTML/CSS Labs
+Project Intros
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Git Lab: Part I
+due
+(in class)</t>
     </r>
   </si>
 </sst>
@@ -1675,70 +1675,70 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2050,8 +2050,8 @@
   </sheetPr>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2073,17 +2073,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="149" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
-      <c r="H1" s="150"/>
-      <c r="I1" s="151"/>
+      <c r="A1" s="133" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="135"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2113,10 +2113,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="141">
+      <c r="A3" s="138">
         <v>15</v>
       </c>
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="147" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="67">
@@ -2148,8 +2148,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="75.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="145"/>
-      <c r="B4" s="153"/>
+      <c r="A4" s="137"/>
+      <c r="B4" s="148"/>
       <c r="C4" s="69" t="s">
         <v>7</v>
       </c>
@@ -2170,17 +2170,17 @@
       </c>
       <c r="G4" s="37"/>
       <c r="H4" s="36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="145">
+      <c r="A5" s="137">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="138" t="s">
-        <v>33</v>
+      <c r="B5" s="142" t="s">
+        <v>31</v>
       </c>
       <c r="C5" s="7">
         <f>I3 + 1</f>
@@ -2211,30 +2211,30 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="146.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="142"/>
-      <c r="B6" s="137"/>
+      <c r="A6" s="139"/>
+      <c r="B6" s="143"/>
       <c r="C6" s="123" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="132" t="s">
         <v>72</v>
-      </c>
-      <c r="D6" s="132" t="s">
-        <v>75</v>
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="124" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G6" s="48"/>
       <c r="H6" s="47" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I6" s="107"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="146">
+      <c r="A7" s="140">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="133" t="s">
+      <c r="B7" s="144" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="38">
@@ -2266,33 +2266,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="87.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="139"/>
-      <c r="B8" s="135"/>
+    <row r="8" spans="1:18" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="141"/>
+      <c r="B8" s="145"/>
       <c r="C8" s="30" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="12" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="G8" s="27"/>
       <c r="H8" s="10" t="s">
         <v>29</v>
       </c>
       <c r="I8" s="108" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="139">
+      <c r="A9" s="141">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="135"/>
+      <c r="B9" s="145"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2330,13 +2330,13 @@
       <c r="R9" s="117"/>
     </row>
     <row r="10" spans="1:18" ht="80.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="139"/>
-      <c r="B10" s="135"/>
+      <c r="A10" s="141"/>
+      <c r="B10" s="145"/>
       <c r="C10" s="109" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="10" t="s">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I10" s="13"/>
       <c r="L10" s="25"/>
@@ -2356,11 +2356,11 @@
       <c r="R10" s="118"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="139">
+      <c r="A11" s="141">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="145"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2398,21 +2398,21 @@
       <c r="R11" s="117"/>
     </row>
     <row r="12" spans="1:18" ht="90.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="139"/>
-      <c r="B12" s="135"/>
+      <c r="A12" s="141"/>
+      <c r="B12" s="145"/>
       <c r="C12" s="126"/>
       <c r="D12" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" s="125" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G12" s="42"/>
       <c r="H12" s="49" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I12" s="78"/>
       <c r="L12" s="25"/>
@@ -2424,12 +2424,12 @@
       <c r="R12" s="118"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="139">
+      <c r="A13" s="141">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="154" t="s">
-        <v>34</v>
+      <c r="B13" s="149" t="s">
+        <v>32</v>
       </c>
       <c r="C13" s="17">
         <f>I11 + 1</f>
@@ -2467,24 +2467,24 @@
       <c r="R13" s="119"/>
     </row>
     <row r="14" spans="1:18" ht="108.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="140"/>
-      <c r="B14" s="134"/>
+      <c r="A14" s="146"/>
+      <c r="B14" s="150"/>
       <c r="C14" s="29"/>
       <c r="D14" s="128" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="90"/>
       <c r="F14" s="43" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G14" s="89" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H14" s="84" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I14" s="85" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L14" s="119"/>
       <c r="M14" s="25"/>
@@ -2495,11 +2495,11 @@
       <c r="R14" s="119"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="141">
+      <c r="A15" s="138">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="142" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="67">
@@ -2532,23 +2532,23 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="142"/>
-      <c r="B16" s="137"/>
+      <c r="A16" s="139"/>
+      <c r="B16" s="143"/>
       <c r="C16" s="86" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E16" s="64" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G16" s="93"/>
       <c r="H16" s="64" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I16" s="94"/>
     </row>
@@ -2572,19 +2572,19 @@
         <v>16</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F19" s="32" t="s">
         <v>17</v>
       </c>
       <c r="G19" s="131" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H19" s="33" t="s">
         <v>18</v>
       </c>
       <c r="I19" s="63" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:18" s="122" customFormat="1" ht="21.4" thickTop="1" x14ac:dyDescent="0.45">
@@ -2610,19 +2610,19 @@
       <c r="I21" s="119"/>
     </row>
     <row r="22" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="149" t="str">
+      <c r="A22" s="133" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
 (as of 1-30-2024, subject to change)</v>
       </c>
-      <c r="B22" s="150"/>
-      <c r="C22" s="150"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="150"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="150"/>
-      <c r="H22" s="150"/>
-      <c r="I22" s="151"/>
+      <c r="B22" s="134"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="134"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="134"/>
+      <c r="G22" s="134"/>
+      <c r="H22" s="134"/>
+      <c r="I22" s="135"/>
     </row>
     <row r="23" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="str">
@@ -2660,11 +2660,11 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="152">
+      <c r="A24" s="136">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B24" s="138" t="s">
+      <c r="B24" s="142" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="95">
@@ -2704,15 +2704,15 @@
       <c r="R24" s="117"/>
     </row>
     <row r="25" spans="1:18" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="145"/>
-      <c r="B25" s="138"/>
+      <c r="A25" s="137"/>
+      <c r="B25" s="142"/>
       <c r="C25" s="51"/>
       <c r="D25" s="22" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6" t="s">
@@ -2728,11 +2728,11 @@
       <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="145">
+      <c r="A26" s="137">
         <f>A24 - 1</f>
         <v>7</v>
       </c>
-      <c r="B26" s="138"/>
+      <c r="B26" s="142"/>
       <c r="C26" s="7">
         <f>I24 + 1</f>
         <v>17</v>
@@ -2770,26 +2770,26 @@
       <c r="R26" s="117"/>
     </row>
     <row r="27" spans="1:18" ht="129.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="145"/>
-      <c r="B27" s="138"/>
+      <c r="A27" s="137"/>
+      <c r="B27" s="142"/>
       <c r="C27" s="116"/>
       <c r="D27" s="26" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="129" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="110" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="110" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" s="36" t="s">
-        <v>67</v>
-      </c>
       <c r="I27" s="115" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="117"/>
@@ -2800,11 +2800,11 @@
       <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="145">
+      <c r="A28" s="137">
         <f>A26 - 1</f>
         <v>6</v>
       </c>
-      <c r="B28" s="138"/>
+      <c r="B28" s="142"/>
       <c r="C28" s="7">
         <f>I26 + 1</f>
         <v>24</v>
@@ -2842,24 +2842,24 @@
       <c r="R28" s="117"/>
     </row>
     <row r="29" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="142"/>
-      <c r="B29" s="137"/>
+      <c r="A29" s="139"/>
+      <c r="B29" s="143"/>
       <c r="C29" s="111"/>
       <c r="D29" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="96"/>
       <c r="H29" s="72" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I29" s="114" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L29" s="25"/>
       <c r="M29" s="117"/>
@@ -2870,12 +2870,12 @@
       <c r="R29" s="25"/>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="146">
+      <c r="A30" s="140">
         <f>A28 -1</f>
         <v>5</v>
       </c>
-      <c r="B30" s="133" t="s">
-        <v>41</v>
+      <c r="B30" s="144" t="s">
+        <v>39</v>
       </c>
       <c r="C30" s="102">
         <f>I28 + 1</f>
@@ -2906,32 +2906,32 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="147"/>
-      <c r="B31" s="134"/>
+      <c r="A31" s="151"/>
+      <c r="B31" s="150"/>
       <c r="C31" s="127" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D31" s="104" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G31" s="79"/>
       <c r="H31" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I31" s="28"/>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="148">
+      <c r="A32" s="152">
         <f>A30 -1</f>
         <v>4</v>
       </c>
-      <c r="B32" s="133" t="s">
+      <c r="B32" s="144" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="60">
@@ -2964,30 +2964,30 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="139"/>
-      <c r="B33" s="135"/>
+      <c r="A33" s="141"/>
+      <c r="B33" s="145"/>
       <c r="C33" s="29"/>
       <c r="D33" s="112" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="113" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G33" s="27"/>
       <c r="H33" s="106" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="139">
+      <c r="A34" s="141">
         <f>A32 -1</f>
         <v>3</v>
       </c>
-      <c r="B34" s="135"/>
+      <c r="B34" s="145"/>
       <c r="C34" s="27">
         <f>I32 + 1</f>
         <v>14</v>
@@ -3018,8 +3018,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="139"/>
-      <c r="B35" s="135"/>
+      <c r="A35" s="141"/>
+      <c r="B35" s="145"/>
       <c r="C35" s="29"/>
       <c r="D35" s="105" t="s">
         <v>6</v>
@@ -3035,11 +3035,11 @@
       <c r="I35" s="28"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="139">
+      <c r="A36" s="141">
         <f>A34 -1</f>
         <v>2</v>
       </c>
-      <c r="B36" s="135"/>
+      <c r="B36" s="145"/>
       <c r="C36" s="29">
         <f>I34 + 1</f>
         <v>21</v>
@@ -3070,8 +3070,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="140"/>
-      <c r="B37" s="134"/>
+      <c r="A37" s="146"/>
+      <c r="B37" s="150"/>
       <c r="C37" s="58"/>
       <c r="D37" s="43" t="s">
         <v>24</v>
@@ -3087,12 +3087,12 @@
       <c r="I37" s="41"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="141">
+      <c r="A38" s="138">
         <f>A36 -1</f>
         <v>1</v>
       </c>
-      <c r="B38" s="136" t="s">
-        <v>42</v>
+      <c r="B38" s="147" t="s">
+        <v>40</v>
       </c>
       <c r="C38" s="17">
         <f>I36 + 1</f>
@@ -3123,8 +3123,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="142"/>
-      <c r="B39" s="137"/>
+      <c r="A39" s="139"/>
+      <c r="B39" s="143"/>
       <c r="C39" s="99"/>
       <c r="D39" s="49" t="s">
         <v>6</v>
@@ -3135,17 +3135,17 @@
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I39" s="130" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="143" t="s">
+      <c r="A40" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="138" t="s">
+      <c r="B40" s="142" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="20">
@@ -3178,17 +3178,17 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="144"/>
-      <c r="B41" s="137"/>
+      <c r="A41" s="154"/>
+      <c r="B41" s="143"/>
       <c r="C41" s="61" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E41" s="62"/>
       <c r="F41" s="23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G41" s="21"/>
       <c r="H41" s="76"/>
@@ -3197,6 +3197,18 @@
     <row r="42" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A3:A4"/>
@@ -3213,18 +3225,6 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>

</xml_diff>

<commit_message>
changes proposal due dates, and added news
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar.xlsx
+++ b/CS320-Spring2024Calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E57E6D-05A1-4E7F-BC48-22C1FDBFAA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5F0A04-F8F3-4EAB-9023-B063CF472D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="878" windowWidth="23520" windowHeight="14572" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68" yWindow="577" windowWidth="27037" windowHeight="14573" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp24" sheetId="1" r:id="rId1"/>
@@ -464,10 +464,6 @@
     </r>
   </si>
   <si>
-    <t>A01: Team Project Proposal due Noon
-(Marmoset)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Review ChatPT and HTML/CSS Labs
 Project Intros
@@ -543,10 +539,6 @@
     <t>Final Prepararion for A06 submission and Team Milestone 1</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2024 Schedule
-(as of 2-6-2024, subject to change)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lab 2a: Web Apps Lab02a due
 Mon, 2-19-24
 -------------&gt;&gt;&gt;&gt;
@@ -558,6 +550,16 @@
     <t>Lecture 4: Web
 Applications II
 Web Applications Labs Review</t>
+  </si>
+  <si>
+    <t>A01: Team Project Proposal due 7:00a, 
+Wed, 2-14-24
+---------&gt;&gt;&gt;&gt;
+(Marmoset)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2024 Schedule
+(as of 2-7-2024, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1579,9 +1581,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1659,35 +1658,65 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1696,35 +1725,11 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2035,8 +2040,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2058,17 +2063,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="150" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="152"/>
+      <c r="A1" s="133" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="135"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2098,10 +2103,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="142">
+      <c r="A3" s="138">
         <v>15</v>
       </c>
-      <c r="B3" s="137" t="s">
+      <c r="B3" s="147" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="67">
@@ -2133,8 +2138,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="75.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="146"/>
-      <c r="B4" s="154"/>
+      <c r="A4" s="137"/>
+      <c r="B4" s="148"/>
       <c r="C4" s="69" t="s">
         <v>7</v>
       </c>
@@ -2160,11 +2165,11 @@
       <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="146">
+      <c r="A5" s="137">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="142" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="7">
@@ -2196,16 +2201,16 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="146.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="143"/>
-      <c r="B6" s="138"/>
-      <c r="C6" s="122" t="s">
+      <c r="A6" s="139"/>
+      <c r="B6" s="143"/>
+      <c r="C6" s="121" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="128" t="s">
+      <c r="D6" s="127" t="s">
         <v>61</v>
       </c>
       <c r="E6" s="57"/>
-      <c r="F6" s="123" t="s">
+      <c r="F6" s="122" t="s">
         <v>62</v>
       </c>
       <c r="G6" s="48"/>
@@ -2215,11 +2220,11 @@
       <c r="I6" s="106"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="147">
+      <c r="A7" s="140">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="144" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="38">
@@ -2252,13 +2257,13 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="140"/>
-      <c r="B8" s="136"/>
+      <c r="A8" s="141"/>
+      <c r="B8" s="145"/>
       <c r="C8" s="30" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="12" t="s">
@@ -2266,18 +2271,16 @@
       </c>
       <c r="G8" s="27"/>
       <c r="H8" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="107" t="s">
-        <v>40</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="I8" s="156"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="140">
+      <c r="A9" s="141">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="136"/>
+      <c r="B9" s="145"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2306,46 +2309,48 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L9" s="116"/>
-      <c r="M9" s="116"/>
-      <c r="N9" s="116"/>
-      <c r="O9" s="116"/>
-      <c r="P9" s="116"/>
-      <c r="Q9" s="116"/>
-      <c r="R9" s="116"/>
+      <c r="L9" s="115"/>
+      <c r="M9" s="115"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="115"/>
+      <c r="P9" s="115"/>
+      <c r="Q9" s="115"/>
+      <c r="R9" s="115"/>
     </row>
     <row r="10" spans="1:18" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="140"/>
-      <c r="B10" s="136"/>
-      <c r="C10" s="108" t="s">
-        <v>65</v>
+      <c r="A10" s="141"/>
+      <c r="B10" s="145"/>
+      <c r="C10" s="155" t="s">
+        <v>40</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="107" t="s">
+        <v>74</v>
+      </c>
       <c r="F10" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I10" s="13"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="116"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="116"/>
-      <c r="P10" s="117"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="117"/>
+      <c r="M10" s="115"/>
+      <c r="N10" s="116"/>
+      <c r="O10" s="115"/>
+      <c r="P10" s="116"/>
+      <c r="Q10" s="115"/>
+      <c r="R10" s="116"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="140">
+      <c r="A11" s="141">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="136"/>
+      <c r="B11" s="145"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2374,46 +2379,46 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="L11" s="116"/>
-      <c r="M11" s="116"/>
-      <c r="N11" s="116"/>
-      <c r="O11" s="116"/>
-      <c r="P11" s="116"/>
-      <c r="Q11" s="116"/>
-      <c r="R11" s="116"/>
+      <c r="L11" s="115"/>
+      <c r="M11" s="115"/>
+      <c r="N11" s="115"/>
+      <c r="O11" s="115"/>
+      <c r="P11" s="115"/>
+      <c r="Q11" s="115"/>
+      <c r="R11" s="115"/>
     </row>
     <row r="12" spans="1:18" ht="97.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="140"/>
-      <c r="B12" s="136"/>
+      <c r="A12" s="141"/>
+      <c r="B12" s="145"/>
       <c r="C12" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="133"/>
+      <c r="E12" s="132"/>
       <c r="F12" s="44" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="42"/>
-      <c r="H12" s="129" t="s">
-        <v>69</v>
+      <c r="H12" s="128" t="s">
+        <v>68</v>
       </c>
       <c r="I12" s="78"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="116"/>
-      <c r="N12" s="116"/>
-      <c r="O12" s="116"/>
-      <c r="P12" s="117"/>
-      <c r="Q12" s="116"/>
-      <c r="R12" s="117"/>
+      <c r="M12" s="115"/>
+      <c r="N12" s="115"/>
+      <c r="O12" s="115"/>
+      <c r="P12" s="116"/>
+      <c r="Q12" s="115"/>
+      <c r="R12" s="116"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="140">
+      <c r="A13" s="141">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="149" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="17">
@@ -2443,23 +2448,23 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L13" s="116"/>
-      <c r="M13" s="116"/>
-      <c r="N13" s="116"/>
-      <c r="O13" s="116"/>
-      <c r="P13" s="116"/>
-      <c r="Q13" s="116"/>
-      <c r="R13" s="118"/>
+      <c r="L13" s="115"/>
+      <c r="M13" s="115"/>
+      <c r="N13" s="115"/>
+      <c r="O13" s="115"/>
+      <c r="P13" s="115"/>
+      <c r="Q13" s="115"/>
+      <c r="R13" s="117"/>
     </row>
     <row r="14" spans="1:18" ht="125.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="141"/>
-      <c r="B14" s="135"/>
+      <c r="A14" s="146"/>
+      <c r="B14" s="150"/>
       <c r="C14" s="29"/>
-      <c r="D14" s="131" t="s">
-        <v>70</v>
+      <c r="D14" s="130" t="s">
+        <v>69</v>
       </c>
       <c r="E14" s="90"/>
-      <c r="F14" s="130" t="s">
+      <c r="F14" s="129" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="89" t="s">
@@ -2471,20 +2476,20 @@
       <c r="I14" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="118"/>
+      <c r="L14" s="117"/>
       <c r="M14" s="25"/>
-      <c r="N14" s="119"/>
-      <c r="O14" s="116"/>
-      <c r="P14" s="118"/>
-      <c r="Q14" s="116"/>
-      <c r="R14" s="118"/>
+      <c r="N14" s="118"/>
+      <c r="O14" s="115"/>
+      <c r="P14" s="117"/>
+      <c r="Q14" s="115"/>
+      <c r="R14" s="117"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="142">
+      <c r="A15" s="138">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="139" t="s">
+      <c r="B15" s="142" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="67">
@@ -2517,13 +2522,13 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="103.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="143"/>
-      <c r="B16" s="138"/>
+      <c r="A16" s="139"/>
+      <c r="B16" s="143"/>
       <c r="C16" s="86" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E16" s="64" t="s">
         <v>28</v>
@@ -2571,7 +2576,7 @@
       <c r="F18" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="127" t="s">
+      <c r="G18" s="126" t="s">
         <v>58</v>
       </c>
       <c r="H18" s="33" t="s">
@@ -2581,31 +2586,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="121" customFormat="1" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="120"/>
+    <row r="19" spans="1:18" s="120" customFormat="1" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="119"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
-      <c r="D19" s="118"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="118"/>
-      <c r="G19" s="118"/>
-      <c r="H19" s="118"/>
-      <c r="I19" s="118"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="117"/>
     </row>
     <row r="20" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="150" t="str">
+      <c r="A20" s="133" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
-(as of 2-6-2024, subject to change)</v>
-      </c>
-      <c r="B20" s="151"/>
-      <c r="C20" s="151"/>
-      <c r="D20" s="151"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="151"/>
-      <c r="G20" s="151"/>
-      <c r="H20" s="151"/>
-      <c r="I20" s="152"/>
+(as of 2-7-2024, subject to change)</v>
+      </c>
+      <c r="B20" s="134"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="134"/>
+      <c r="F20" s="134"/>
+      <c r="G20" s="134"/>
+      <c r="H20" s="134"/>
+      <c r="I20" s="135"/>
     </row>
     <row r="21" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="str">
@@ -2643,11 +2648,11 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="153">
+      <c r="A22" s="136">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B22" s="139" t="s">
+      <c r="B22" s="142" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="95">
@@ -2678,20 +2683,20 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="L22" s="118"/>
-      <c r="M22" s="116"/>
-      <c r="N22" s="116"/>
-      <c r="O22" s="116"/>
-      <c r="P22" s="116"/>
-      <c r="Q22" s="116"/>
-      <c r="R22" s="116"/>
+      <c r="L22" s="117"/>
+      <c r="M22" s="115"/>
+      <c r="N22" s="115"/>
+      <c r="O22" s="115"/>
+      <c r="P22" s="115"/>
+      <c r="Q22" s="115"/>
+      <c r="R22" s="115"/>
     </row>
     <row r="23" spans="1:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="146"/>
-      <c r="B23" s="139"/>
+      <c r="A23" s="137"/>
+      <c r="B23" s="142"/>
       <c r="C23" s="51"/>
       <c r="D23" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E23" s="50" t="s">
         <v>55</v>
@@ -2704,20 +2709,20 @@
         <v>15</v>
       </c>
       <c r="I23" s="35"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="116"/>
-      <c r="N23" s="116"/>
-      <c r="O23" s="116"/>
-      <c r="P23" s="116"/>
-      <c r="Q23" s="116"/>
+      <c r="L23" s="115"/>
+      <c r="M23" s="115"/>
+      <c r="N23" s="115"/>
+      <c r="O23" s="115"/>
+      <c r="P23" s="115"/>
+      <c r="Q23" s="115"/>
       <c r="R23" s="25"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="146">
+      <c r="A24" s="137">
         <f>A22 - 1</f>
         <v>7</v>
       </c>
-      <c r="B24" s="139"/>
+      <c r="B24" s="142"/>
       <c r="C24" s="7">
         <f>I22 + 1</f>
         <v>17</v>
@@ -2746,50 +2751,50 @@
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="L24" s="116"/>
-      <c r="M24" s="116"/>
-      <c r="N24" s="116"/>
-      <c r="O24" s="116"/>
-      <c r="P24" s="116"/>
-      <c r="Q24" s="116"/>
-      <c r="R24" s="116"/>
+      <c r="L24" s="115"/>
+      <c r="M24" s="115"/>
+      <c r="N24" s="115"/>
+      <c r="O24" s="115"/>
+      <c r="P24" s="115"/>
+      <c r="Q24" s="115"/>
+      <c r="R24" s="115"/>
     </row>
     <row r="25" spans="1:18" ht="124.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="146"/>
-      <c r="B25" s="139"/>
-      <c r="C25" s="115"/>
+      <c r="A25" s="137"/>
+      <c r="B25" s="142"/>
+      <c r="C25" s="114"/>
       <c r="D25" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="125" t="s">
+      <c r="E25" s="124" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="109" t="s">
+      <c r="G25" s="108" t="s">
         <v>41</v>
       </c>
       <c r="H25" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="I25" s="114" t="s">
+      <c r="I25" s="113" t="s">
         <v>42</v>
       </c>
       <c r="L25" s="25"/>
-      <c r="M25" s="116"/>
-      <c r="N25" s="118"/>
-      <c r="O25" s="116"/>
-      <c r="P25" s="118"/>
-      <c r="Q25" s="116"/>
+      <c r="M25" s="115"/>
+      <c r="N25" s="117"/>
+      <c r="O25" s="115"/>
+      <c r="P25" s="117"/>
+      <c r="Q25" s="115"/>
       <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="146">
+      <c r="A26" s="137">
         <f>A24 - 1</f>
         <v>6</v>
       </c>
-      <c r="B26" s="139"/>
+      <c r="B26" s="142"/>
       <c r="C26" s="7">
         <f>I24 + 1</f>
         <v>24</v>
@@ -2818,18 +2823,18 @@
         <f t="shared" ref="I26" si="9">H26 + 1</f>
         <v>30</v>
       </c>
-      <c r="L26" s="116"/>
-      <c r="M26" s="116"/>
-      <c r="N26" s="116"/>
-      <c r="O26" s="116"/>
-      <c r="P26" s="116"/>
-      <c r="Q26" s="116"/>
-      <c r="R26" s="116"/>
+      <c r="L26" s="115"/>
+      <c r="M26" s="115"/>
+      <c r="N26" s="115"/>
+      <c r="O26" s="115"/>
+      <c r="P26" s="115"/>
+      <c r="Q26" s="115"/>
+      <c r="R26" s="115"/>
     </row>
     <row r="27" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="143"/>
-      <c r="B27" s="138"/>
-      <c r="C27" s="110"/>
+      <c r="A27" s="139"/>
+      <c r="B27" s="143"/>
+      <c r="C27" s="109"/>
       <c r="D27" s="9" t="s">
         <v>22</v>
       </c>
@@ -2837,29 +2842,29 @@
       <c r="F27" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="132" t="s">
+      <c r="G27" s="131" t="s">
         <v>54</v>
       </c>
       <c r="H27" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="I27" s="113" t="s">
+      <c r="I27" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="L27" s="116"/>
-      <c r="M27" s="116"/>
+      <c r="L27" s="115"/>
+      <c r="M27" s="115"/>
       <c r="N27" s="25"/>
-      <c r="O27" s="116"/>
+      <c r="O27" s="115"/>
       <c r="P27" s="25"/>
-      <c r="Q27" s="118"/>
+      <c r="Q27" s="117"/>
       <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="147">
+      <c r="A28" s="140">
         <f>A26 -1</f>
         <v>5</v>
       </c>
-      <c r="B28" s="134" t="s">
+      <c r="B28" s="144" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="101">
@@ -2891,9 +2896,9 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="148"/>
-      <c r="B29" s="135"/>
-      <c r="C29" s="124" t="s">
+      <c r="A29" s="151"/>
+      <c r="B29" s="150"/>
+      <c r="C29" s="123" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="103" t="s">
@@ -2912,11 +2917,11 @@
       <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="149">
+      <c r="A30" s="152">
         <f>A28 -1</f>
         <v>4</v>
       </c>
-      <c r="B30" s="134" t="s">
+      <c r="B30" s="144" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="60">
@@ -2949,13 +2954,13 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="140"/>
-      <c r="B31" s="136"/>
+      <c r="A31" s="141"/>
+      <c r="B31" s="145"/>
       <c r="C31" s="29"/>
-      <c r="D31" s="111" t="s">
+      <c r="D31" s="110" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="112" t="s">
+      <c r="E31" s="111" t="s">
         <v>52</v>
       </c>
       <c r="F31" s="12" t="s">
@@ -2968,11 +2973,11 @@
       <c r="I31" s="28"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="140">
+      <c r="A32" s="141">
         <f>A30 -1</f>
         <v>3</v>
       </c>
-      <c r="B32" s="136"/>
+      <c r="B32" s="145"/>
       <c r="C32" s="27">
         <f>I30 + 1</f>
         <v>14</v>
@@ -3003,8 +3008,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="140"/>
-      <c r="B33" s="136"/>
+      <c r="A33" s="141"/>
+      <c r="B33" s="145"/>
       <c r="C33" s="29"/>
       <c r="D33" s="104" t="s">
         <v>6</v>
@@ -3020,11 +3025,11 @@
       <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="140">
+      <c r="A34" s="141">
         <f>A32 -1</f>
         <v>2</v>
       </c>
-      <c r="B34" s="136"/>
+      <c r="B34" s="145"/>
       <c r="C34" s="29">
         <f>I32 + 1</f>
         <v>21</v>
@@ -3055,8 +3060,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="141"/>
-      <c r="B35" s="135"/>
+      <c r="A35" s="146"/>
+      <c r="B35" s="150"/>
       <c r="C35" s="58"/>
       <c r="D35" s="43" t="s">
         <v>23</v>
@@ -3072,11 +3077,11 @@
       <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="142">
+      <c r="A36" s="138">
         <f>A34 -1</f>
         <v>1</v>
       </c>
-      <c r="B36" s="137" t="s">
+      <c r="B36" s="147" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="17">
@@ -3108,8 +3113,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="143"/>
-      <c r="B37" s="138"/>
+      <c r="A37" s="139"/>
+      <c r="B37" s="143"/>
       <c r="C37" s="98"/>
       <c r="D37" s="49" t="s">
         <v>6</v>
@@ -3122,15 +3127,15 @@
       <c r="H37" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I37" s="126" t="s">
+      <c r="I37" s="125" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="144" t="s">
+      <c r="A38" s="153" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="139" t="s">
+      <c r="B38" s="142" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="20">
@@ -3163,8 +3168,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="145"/>
-      <c r="B39" s="138"/>
+      <c r="A39" s="154"/>
+      <c r="B39" s="143"/>
       <c r="C39" s="61" t="s">
         <v>44</v>
       </c>
@@ -3182,6 +3187,18 @@
     <row r="40" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A3:A4"/>
@@ -3198,18 +3215,6 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>

</xml_diff>

<commit_message>
schedule and calendars updates
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar.xlsx
+++ b/CS320-Spring2024Calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5F0A04-F8F3-4EAB-9023-B063CF472D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B808FC54-3AFA-4D46-B20E-BBF90E46B4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68" yWindow="577" windowWidth="27037" windowHeight="14573" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10245" yWindow="405" windowWidth="18510" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp24" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Monday</t>
   </si>
@@ -274,12 +274,6 @@
   </si>
   <si>
     <t>A08: Team Report due Noon
-(Marmoset)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-A09: Individual  Report 
-due Noon
 (Marmoset)</t>
   </si>
   <si>
@@ -559,7 +553,18 @@
   </si>
   <si>
     <t>CS320: SW Engineering - Spring 2024 Schedule
-(as of 2-7-2024, subject to change)</t>
+(as of 2-17-2024, subject to change)</t>
+  </si>
+  <si>
+    <t>(Marmoset)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A09: Individual  Report 
+due 4-10-24
+by 7:00a
+-----&gt;&gt;&gt;&gt;&gt;
+(Marmoset)</t>
   </si>
 </sst>
 </file>
@@ -1632,9 +1637,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1659,50 +1661,71 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1710,25 +1733,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2040,8 +2045,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2063,17 +2068,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="133" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="135"/>
+      <c r="A1" s="150" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="152"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2103,10 +2108,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="138">
+      <c r="A3" s="142">
         <v>15</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="137" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="67">
@@ -2138,8 +2143,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="75.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="137"/>
-      <c r="B4" s="148"/>
+      <c r="A4" s="146"/>
+      <c r="B4" s="154"/>
       <c r="C4" s="69" t="s">
         <v>7</v>
       </c>
@@ -2160,16 +2165,16 @@
       </c>
       <c r="G4" s="37"/>
       <c r="H4" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="137">
+      <c r="A5" s="146">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="142" t="s">
+      <c r="B5" s="139" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="7">
@@ -2201,30 +2206,30 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="146.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="139"/>
-      <c r="B6" s="143"/>
+      <c r="A6" s="143"/>
+      <c r="B6" s="138"/>
       <c r="C6" s="121" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="127" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="D6" s="126" t="s">
+        <v>60</v>
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="122" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="48"/>
       <c r="H6" s="47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I6" s="106"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="140">
+      <c r="A7" s="147">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="144" t="s">
+      <c r="B7" s="134" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="38">
@@ -2257,30 +2262,30 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="141"/>
-      <c r="B8" s="145"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="136"/>
       <c r="C8" s="30" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="27"/>
       <c r="H8" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" s="156"/>
+        <v>72</v>
+      </c>
+      <c r="I8" s="133"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="141">
+      <c r="A9" s="140">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="145"/>
+      <c r="B9" s="136"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2318,23 +2323,23 @@
       <c r="R9" s="115"/>
     </row>
     <row r="10" spans="1:18" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="141"/>
-      <c r="B10" s="145"/>
-      <c r="C10" s="155" t="s">
+      <c r="A10" s="140"/>
+      <c r="B10" s="136"/>
+      <c r="C10" s="132" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E10" s="107" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I10" s="13"/>
       <c r="L10" s="25"/>
@@ -2346,11 +2351,11 @@
       <c r="R10" s="116"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="141">
+      <c r="A11" s="140">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="145"/>
+      <c r="B11" s="136"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2388,21 +2393,21 @@
       <c r="R11" s="115"/>
     </row>
     <row r="12" spans="1:18" ht="97.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="141"/>
-      <c r="B12" s="145"/>
+      <c r="A12" s="140"/>
+      <c r="B12" s="136"/>
       <c r="C12" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="132"/>
+      <c r="E12" s="131"/>
       <c r="F12" s="44" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="42"/>
-      <c r="H12" s="128" t="s">
-        <v>68</v>
+      <c r="H12" s="127" t="s">
+        <v>67</v>
       </c>
       <c r="I12" s="78"/>
       <c r="L12" s="25"/>
@@ -2414,11 +2419,11 @@
       <c r="R12" s="116"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="141">
+      <c r="A13" s="140">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="149" t="s">
+      <c r="B13" s="155" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="17">
@@ -2457,14 +2462,14 @@
       <c r="R13" s="117"/>
     </row>
     <row r="14" spans="1:18" ht="125.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="146"/>
-      <c r="B14" s="150"/>
+      <c r="A14" s="141"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="29"/>
-      <c r="D14" s="130" t="s">
-        <v>69</v>
+      <c r="D14" s="129" t="s">
+        <v>68</v>
       </c>
       <c r="E14" s="90"/>
-      <c r="F14" s="129" t="s">
+      <c r="F14" s="128" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="89" t="s">
@@ -2485,11 +2490,11 @@
       <c r="R14" s="117"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="138">
+      <c r="A15" s="142">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="142" t="s">
+      <c r="B15" s="139" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="67">
@@ -2522,13 +2527,13 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="103.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="139"/>
-      <c r="B16" s="143"/>
+      <c r="A16" s="143"/>
+      <c r="B16" s="138"/>
       <c r="C16" s="86" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" s="64" t="s">
         <v>28</v>
@@ -2571,13 +2576,13 @@
         <v>16</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="126" t="s">
-        <v>58</v>
+      <c r="G18" s="125" t="s">
+        <v>57</v>
       </c>
       <c r="H18" s="33" t="s">
         <v>18</v>
@@ -2598,19 +2603,19 @@
       <c r="I19" s="117"/>
     </row>
     <row r="20" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="133" t="str">
+      <c r="A20" s="150" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
-(as of 2-7-2024, subject to change)</v>
-      </c>
-      <c r="B20" s="134"/>
-      <c r="C20" s="134"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="134"/>
-      <c r="F20" s="134"/>
-      <c r="G20" s="134"/>
-      <c r="H20" s="134"/>
-      <c r="I20" s="135"/>
+(as of 2-17-2024, subject to change)</v>
+      </c>
+      <c r="B20" s="151"/>
+      <c r="C20" s="151"/>
+      <c r="D20" s="151"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="151"/>
+      <c r="I20" s="152"/>
     </row>
     <row r="21" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="str">
@@ -2648,11 +2653,11 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="136">
+      <c r="A22" s="153">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B22" s="142" t="s">
+      <c r="B22" s="139" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="95">
@@ -2692,14 +2697,14 @@
       <c r="R22" s="115"/>
     </row>
     <row r="23" spans="1:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="137"/>
-      <c r="B23" s="142"/>
+      <c r="A23" s="146"/>
+      <c r="B23" s="139"/>
       <c r="C23" s="51"/>
       <c r="D23" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="50" t="s">
-        <v>55</v>
+        <v>70</v>
+      </c>
+      <c r="E23" s="107" t="s">
+        <v>54</v>
       </c>
       <c r="F23" s="22" t="s">
         <v>14</v>
@@ -2718,11 +2723,11 @@
       <c r="R23" s="25"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="137">
+      <c r="A24" s="146">
         <f>A22 - 1</f>
         <v>7</v>
       </c>
-      <c r="B24" s="142"/>
+      <c r="B24" s="139"/>
       <c r="C24" s="7">
         <f>I22 + 1</f>
         <v>17</v>
@@ -2760,15 +2765,13 @@
       <c r="R24" s="115"/>
     </row>
     <row r="25" spans="1:18" ht="124.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="137"/>
-      <c r="B25" s="142"/>
+      <c r="A25" s="146"/>
+      <c r="B25" s="139"/>
       <c r="C25" s="114"/>
       <c r="D25" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="124" t="s">
-        <v>55</v>
-      </c>
+      <c r="E25" s="156"/>
       <c r="F25" s="55" t="s">
         <v>43</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>41</v>
       </c>
       <c r="H25" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I25" s="113" t="s">
         <v>42</v>
@@ -2790,11 +2793,11 @@
       <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="137">
+      <c r="A26" s="146">
         <f>A24 - 1</f>
         <v>6</v>
       </c>
-      <c r="B26" s="142"/>
+      <c r="B26" s="139"/>
       <c r="C26" s="7">
         <f>I24 + 1</f>
         <v>24</v>
@@ -2832,8 +2835,8 @@
       <c r="R26" s="115"/>
     </row>
     <row r="27" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="139"/>
-      <c r="B27" s="143"/>
+      <c r="A27" s="143"/>
+      <c r="B27" s="138"/>
       <c r="C27" s="109"/>
       <c r="D27" s="9" t="s">
         <v>22</v>
@@ -2842,8 +2845,8 @@
       <c r="F27" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="131" t="s">
-        <v>54</v>
+      <c r="G27" s="130" t="s">
+        <v>53</v>
       </c>
       <c r="H27" s="72" t="s">
         <v>39</v>
@@ -2860,11 +2863,11 @@
       <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="140">
+      <c r="A28" s="147">
         <f>A26 -1</f>
         <v>5</v>
       </c>
-      <c r="B28" s="144" t="s">
+      <c r="B28" s="134" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="101">
@@ -2896,8 +2899,8 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="151"/>
-      <c r="B29" s="150"/>
+      <c r="A29" s="148"/>
+      <c r="B29" s="135"/>
       <c r="C29" s="123" t="s">
         <v>39</v>
       </c>
@@ -2905,7 +2908,7 @@
         <v>39</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>46</v>
@@ -2917,11 +2920,11 @@
       <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="152">
+      <c r="A30" s="149">
         <f>A28 -1</f>
         <v>4</v>
       </c>
-      <c r="B30" s="144" t="s">
+      <c r="B30" s="134" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="60">
@@ -2954,14 +2957,14 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="141"/>
-      <c r="B31" s="145"/>
+      <c r="A31" s="140"/>
+      <c r="B31" s="136"/>
       <c r="C31" s="29"/>
       <c r="D31" s="110" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="111" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>47</v>
@@ -2973,11 +2976,11 @@
       <c r="I31" s="28"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="141">
+      <c r="A32" s="140">
         <f>A30 -1</f>
         <v>3</v>
       </c>
-      <c r="B32" s="145"/>
+      <c r="B32" s="136"/>
       <c r="C32" s="27">
         <f>I30 + 1</f>
         <v>14</v>
@@ -2987,11 +2990,11 @@
         <v>15</v>
       </c>
       <c r="E32" s="12">
-        <f t="shared" ref="E32:I32" si="11">D32 + 1</f>
+        <f>D32 + 1</f>
         <v>16</v>
       </c>
       <c r="F32" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="E32:I32" si="11">E32 + 1</f>
         <v>17</v>
       </c>
       <c r="G32" s="27">
@@ -3008,13 +3011,15 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="141"/>
-      <c r="B33" s="145"/>
+      <c r="A33" s="140"/>
+      <c r="B33" s="136"/>
       <c r="C33" s="29"/>
       <c r="D33" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="11"/>
+      <c r="E33" s="11" t="s">
+        <v>75</v>
+      </c>
       <c r="F33" s="44" t="s">
         <v>6</v>
       </c>
@@ -3025,11 +3030,11 @@
       <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="141">
+      <c r="A34" s="140">
         <f>A32 -1</f>
         <v>2</v>
       </c>
-      <c r="B34" s="145"/>
+      <c r="B34" s="136"/>
       <c r="C34" s="29">
         <f>I32 + 1</f>
         <v>21</v>
@@ -3060,8 +3065,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="146"/>
-      <c r="B35" s="150"/>
+      <c r="A35" s="141"/>
+      <c r="B35" s="135"/>
       <c r="C35" s="58"/>
       <c r="D35" s="43" t="s">
         <v>23</v>
@@ -3077,11 +3082,11 @@
       <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="138">
+      <c r="A36" s="142">
         <f>A34 -1</f>
         <v>1</v>
       </c>
-      <c r="B36" s="147" t="s">
+      <c r="B36" s="137" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="17">
@@ -3113,8 +3118,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="139"/>
-      <c r="B37" s="143"/>
+      <c r="A37" s="143"/>
+      <c r="B37" s="138"/>
       <c r="C37" s="98"/>
       <c r="D37" s="49" t="s">
         <v>6</v>
@@ -3127,15 +3132,15 @@
       <c r="H37" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I37" s="125" t="s">
+      <c r="I37" s="124" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="153" t="s">
+      <c r="A38" s="144" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="142" t="s">
+      <c r="B38" s="139" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="20">
@@ -3168,8 +3173,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="154"/>
-      <c r="B39" s="143"/>
+      <c r="A39" s="145"/>
+      <c r="B39" s="138"/>
       <c r="C39" s="61" t="s">
         <v>44</v>
       </c>
@@ -3187,18 +3192,6 @@
     <row r="40" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A3:A4"/>
@@ -3215,6 +3208,18 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>

</xml_diff>

<commit_message>
updates to assign05 and assign06, plus resources page, and schedules
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar.xlsx
+++ b/CS320-Spring2024Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B808FC54-3AFA-4D46-B20E-BBF90E46B4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774F2687-485F-4B99-A798-2BF59B6D43CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10245" yWindow="405" windowWidth="18510" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
   <si>
     <t>Monday</t>
   </si>
@@ -286,11 +286,6 @@
 Peer Evals
 due Noon
 (Marmoset)</t>
-  </si>
-  <si>
-    <t>A06: Team Domain Analysis and Design
-due Noon
-(Google Doc)</t>
   </si>
   <si>
     <r>
@@ -495,11 +490,58 @@
   </si>
   <si>
     <t>Team Session:
+Team Analysis &amp; Design Model
+Team Git Set-Up
+Team MS1 Prep
+(all in-class)</t>
+  </si>
+  <si>
+    <t>Final Prepararion for A06 submission and Team Milestone 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab 2a: Web Apps Lab02a due
+Mon, 2-19-24
+-------------&gt;&gt;&gt;&gt;
+ (after sign-off)
+(Marmoset)
+</t>
+  </si>
+  <si>
+    <t>Lecture 4: Web
+Applications II
+Web Applications Labs Review</t>
+  </si>
+  <si>
+    <t>A01: Team Project Proposal due 7:00a, 
+Wed, 2-14-24
+---------&gt;&gt;&gt;&gt;
+(Marmoset)</t>
+  </si>
+  <si>
+    <t>(Marmoset)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A09: Individual  Report 
+due 4-10-24
+by 7:00a
+-----&gt;&gt;&gt;&gt;&gt;
+(Marmoset)</t>
+  </si>
+  <si>
+    <t>Team Session:
 Textual Analysis
 (in class)
-A05: Team Use Cases
+A05: Team Draft
+Use Cases
+due in-class
+(Google Doc)</t>
+  </si>
+  <si>
+    <t>A05: Team Final Use Cases
 due Noon
-(Google Doc)</t>
+(Google Doc)
+(Marmoset PDF)</t>
   </si>
   <si>
     <r>
@@ -523,48 +565,14 @@
     </r>
   </si>
   <si>
-    <t>Team Session:
-Team Analysis &amp; Design Model
-Team Git Set-Up
-Team MS1 Prep
-(all in-class)</t>
-  </si>
-  <si>
-    <t>Final Prepararion for A06 submission and Team Milestone 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lab 2a: Web Apps Lab02a due
-Mon, 2-19-24
--------------&gt;&gt;&gt;&gt;
- (after sign-off)
-(Marmoset)
-</t>
-  </si>
-  <si>
-    <t>Lecture 4: Web
-Applications II
-Web Applications Labs Review</t>
-  </si>
-  <si>
-    <t>A01: Team Project Proposal due 7:00a, 
-Wed, 2-14-24
----------&gt;&gt;&gt;&gt;
-(Marmoset)</t>
+    <t>A06: Team Domain Analysis and Design
+due Noon
+(Google Doc)
+(Marmoset PDF)</t>
   </si>
   <si>
     <t>CS320: SW Engineering - Spring 2024 Schedule
-(as of 2-17-2024, subject to change)</t>
-  </si>
-  <si>
-    <t>(Marmoset)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-A09: Individual  Report 
-due 4-10-24
-by 7:00a
------&gt;&gt;&gt;&gt;&gt;
-(Marmoset)</t>
+(as of 2-18-2024, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1646,9 +1654,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1666,35 +1671,68 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1703,37 +1741,10 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2045,8 +2056,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2068,17 +2079,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="150" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="152"/>
+      <c r="A1" s="134" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="136"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2108,10 +2119,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="142">
+      <c r="A3" s="139">
         <v>15</v>
       </c>
-      <c r="B3" s="137" t="s">
+      <c r="B3" s="148" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="67">
@@ -2143,8 +2154,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="75.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="146"/>
-      <c r="B4" s="154"/>
+      <c r="A4" s="138"/>
+      <c r="B4" s="149"/>
       <c r="C4" s="69" t="s">
         <v>7</v>
       </c>
@@ -2165,16 +2176,16 @@
       </c>
       <c r="G4" s="37"/>
       <c r="H4" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="146">
+      <c r="A5" s="138">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="143" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="7">
@@ -2206,30 +2217,30 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="146.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="143"/>
-      <c r="B6" s="138"/>
+      <c r="A6" s="140"/>
+      <c r="B6" s="144"/>
       <c r="C6" s="121" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="126" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="122" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="48"/>
       <c r="H6" s="47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I6" s="106"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="147">
+      <c r="A7" s="141">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="145" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="38">
@@ -2262,30 +2273,30 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="140"/>
-      <c r="B8" s="136"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="146"/>
       <c r="C8" s="30" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G8" s="27"/>
       <c r="H8" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8" s="133"/>
+        <v>69</v>
+      </c>
+      <c r="I8" s="132"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="140">
+      <c r="A9" s="142">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="136"/>
+      <c r="B9" s="146"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2323,23 +2334,23 @@
       <c r="R9" s="115"/>
     </row>
     <row r="10" spans="1:18" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="140"/>
-      <c r="B10" s="136"/>
-      <c r="C10" s="132" t="s">
+      <c r="A10" s="142"/>
+      <c r="B10" s="146"/>
+      <c r="C10" s="131" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E10" s="107" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" s="13"/>
       <c r="L10" s="25"/>
@@ -2351,11 +2362,11 @@
       <c r="R10" s="116"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="140">
+      <c r="A11" s="142">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="136"/>
+      <c r="B11" s="146"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2392,22 +2403,22 @@
       <c r="Q11" s="115"/>
       <c r="R11" s="115"/>
     </row>
-    <row r="12" spans="1:18" ht="97.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="140"/>
-      <c r="B12" s="136"/>
+    <row r="12" spans="1:18" ht="102.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="142"/>
+      <c r="B12" s="146"/>
       <c r="C12" s="30" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="131"/>
+      <c r="E12" s="130"/>
       <c r="F12" s="44" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="42"/>
-      <c r="H12" s="127" t="s">
-        <v>67</v>
+      <c r="H12" s="156" t="s">
+        <v>73</v>
       </c>
       <c r="I12" s="78"/>
       <c r="L12" s="25"/>
@@ -2419,11 +2430,11 @@
       <c r="R12" s="116"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="140">
+      <c r="A13" s="142">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="150" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="17">
@@ -2461,15 +2472,17 @@
       <c r="Q13" s="115"/>
       <c r="R13" s="117"/>
     </row>
-    <row r="14" spans="1:18" ht="125.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="141"/>
-      <c r="B14" s="135"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="129" t="s">
-        <v>68</v>
+    <row r="14" spans="1:18" ht="116.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="147"/>
+      <c r="B14" s="151"/>
+      <c r="C14" s="157" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="128" t="s">
+        <v>75</v>
       </c>
       <c r="E14" s="90"/>
-      <c r="F14" s="128" t="s">
+      <c r="F14" s="127" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="89" t="s">
@@ -2490,11 +2503,11 @@
       <c r="R14" s="117"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="142">
+      <c r="A15" s="139">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="139" t="s">
+      <c r="B15" s="143" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="67">
@@ -2527,13 +2540,13 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="103.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="143"/>
-      <c r="B16" s="138"/>
+      <c r="A16" s="140"/>
+      <c r="B16" s="144"/>
       <c r="C16" s="86" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E16" s="64" t="s">
         <v>28</v>
@@ -2576,13 +2589,13 @@
         <v>16</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18" s="32" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="125" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H18" s="33" t="s">
         <v>18</v>
@@ -2603,19 +2616,19 @@
       <c r="I19" s="117"/>
     </row>
     <row r="20" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="150" t="str">
+      <c r="A20" s="134" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
-(as of 2-17-2024, subject to change)</v>
-      </c>
-      <c r="B20" s="151"/>
-      <c r="C20" s="151"/>
-      <c r="D20" s="151"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="151"/>
-      <c r="G20" s="151"/>
-      <c r="H20" s="151"/>
-      <c r="I20" s="152"/>
+(as of 2-18-2024, subject to change)</v>
+      </c>
+      <c r="B20" s="135"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="135"/>
+      <c r="E20" s="135"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="135"/>
+      <c r="I20" s="136"/>
     </row>
     <row r="21" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="str">
@@ -2653,11 +2666,11 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="153">
+      <c r="A22" s="137">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B22" s="139" t="s">
+      <c r="B22" s="143" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="95">
@@ -2696,15 +2709,15 @@
       <c r="Q22" s="115"/>
       <c r="R22" s="115"/>
     </row>
-    <row r="23" spans="1:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="146"/>
-      <c r="B23" s="139"/>
+    <row r="23" spans="1:18" ht="76.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="138"/>
+      <c r="B23" s="143"/>
       <c r="C23" s="51"/>
       <c r="D23" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E23" s="107" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="F23" s="22" t="s">
         <v>14</v>
@@ -2723,11 +2736,11 @@
       <c r="R23" s="25"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="146">
+      <c r="A24" s="138">
         <f>A22 - 1</f>
         <v>7</v>
       </c>
-      <c r="B24" s="139"/>
+      <c r="B24" s="143"/>
       <c r="C24" s="7">
         <f>I22 + 1</f>
         <v>17</v>
@@ -2765,13 +2778,13 @@
       <c r="R24" s="115"/>
     </row>
     <row r="25" spans="1:18" ht="124.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="146"/>
-      <c r="B25" s="139"/>
+      <c r="A25" s="138"/>
+      <c r="B25" s="143"/>
       <c r="C25" s="114"/>
       <c r="D25" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="156"/>
+      <c r="E25" s="133"/>
       <c r="F25" s="55" t="s">
         <v>43</v>
       </c>
@@ -2779,7 +2792,7 @@
         <v>41</v>
       </c>
       <c r="H25" s="36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I25" s="113" t="s">
         <v>42</v>
@@ -2793,11 +2806,11 @@
       <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="146">
+      <c r="A26" s="138">
         <f>A24 - 1</f>
         <v>6</v>
       </c>
-      <c r="B26" s="139"/>
+      <c r="B26" s="143"/>
       <c r="C26" s="7">
         <f>I24 + 1</f>
         <v>24</v>
@@ -2835,8 +2848,8 @@
       <c r="R26" s="115"/>
     </row>
     <row r="27" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="143"/>
-      <c r="B27" s="138"/>
+      <c r="A27" s="140"/>
+      <c r="B27" s="144"/>
       <c r="C27" s="109"/>
       <c r="D27" s="9" t="s">
         <v>22</v>
@@ -2845,7 +2858,7 @@
       <c r="F27" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="130" t="s">
+      <c r="G27" s="129" t="s">
         <v>53</v>
       </c>
       <c r="H27" s="72" t="s">
@@ -2863,11 +2876,11 @@
       <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="147">
+      <c r="A28" s="141">
         <f>A26 -1</f>
         <v>5</v>
       </c>
-      <c r="B28" s="134" t="s">
+      <c r="B28" s="145" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="101">
@@ -2899,8 +2912,8 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="148"/>
-      <c r="B29" s="135"/>
+      <c r="A29" s="152"/>
+      <c r="B29" s="151"/>
       <c r="C29" s="123" t="s">
         <v>39</v>
       </c>
@@ -2920,11 +2933,11 @@
       <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="149">
+      <c r="A30" s="153">
         <f>A28 -1</f>
         <v>4</v>
       </c>
-      <c r="B30" s="134" t="s">
+      <c r="B30" s="145" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="60">
@@ -2957,14 +2970,14 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="140"/>
-      <c r="B31" s="136"/>
+      <c r="A31" s="142"/>
+      <c r="B31" s="146"/>
       <c r="C31" s="29"/>
       <c r="D31" s="110" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="111" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>47</v>
@@ -2976,11 +2989,11 @@
       <c r="I31" s="28"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="140">
+      <c r="A32" s="142">
         <f>A30 -1</f>
         <v>3</v>
       </c>
-      <c r="B32" s="136"/>
+      <c r="B32" s="146"/>
       <c r="C32" s="27">
         <f>I30 + 1</f>
         <v>14</v>
@@ -2994,7 +3007,7 @@
         <v>16</v>
       </c>
       <c r="F32" s="15">
-        <f t="shared" ref="E32:I32" si="11">E32 + 1</f>
+        <f t="shared" ref="F32:I32" si="11">E32 + 1</f>
         <v>17</v>
       </c>
       <c r="G32" s="27">
@@ -3011,14 +3024,14 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="140"/>
-      <c r="B33" s="136"/>
+      <c r="A33" s="142"/>
+      <c r="B33" s="146"/>
       <c r="C33" s="29"/>
       <c r="D33" s="104" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F33" s="44" t="s">
         <v>6</v>
@@ -3030,11 +3043,11 @@
       <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="140">
+      <c r="A34" s="142">
         <f>A32 -1</f>
         <v>2</v>
       </c>
-      <c r="B34" s="136"/>
+      <c r="B34" s="146"/>
       <c r="C34" s="29">
         <f>I32 + 1</f>
         <v>21</v>
@@ -3065,8 +3078,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="141"/>
-      <c r="B35" s="135"/>
+      <c r="A35" s="147"/>
+      <c r="B35" s="151"/>
       <c r="C35" s="58"/>
       <c r="D35" s="43" t="s">
         <v>23</v>
@@ -3082,11 +3095,11 @@
       <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="142">
+      <c r="A36" s="139">
         <f>A34 -1</f>
         <v>1</v>
       </c>
-      <c r="B36" s="137" t="s">
+      <c r="B36" s="148" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="17">
@@ -3118,8 +3131,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="143"/>
-      <c r="B37" s="138"/>
+      <c r="A37" s="140"/>
+      <c r="B37" s="144"/>
       <c r="C37" s="98"/>
       <c r="D37" s="49" t="s">
         <v>6</v>
@@ -3137,10 +3150,10 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="144" t="s">
+      <c r="A38" s="154" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="139" t="s">
+      <c r="B38" s="143" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="20">
@@ -3173,8 +3186,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="145"/>
-      <c r="B39" s="138"/>
+      <c r="A39" s="155"/>
+      <c r="B39" s="144"/>
       <c r="C39" s="61" t="s">
         <v>44</v>
       </c>
@@ -3192,6 +3205,18 @@
     <row r="40" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A3:A4"/>
@@ -3208,18 +3233,6 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>

</xml_diff>

<commit_message>
moved JDBC lab due date
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar.xlsx
+++ b/CS320-Spring2024Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774F2687-485F-4B99-A798-2BF59B6D43CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8C8BEC-5042-4990-850D-5DC67B5B71EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10245" yWindow="405" windowWidth="18510" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1600,9 +1600,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1610,9 +1607,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1745,6 +1739,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2056,8 +2056,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2079,17 +2079,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="132" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="136"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="134"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2119,10 +2119,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="139">
+      <c r="A3" s="137">
         <v>15</v>
       </c>
-      <c r="B3" s="148" t="s">
+      <c r="B3" s="146" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="67">
@@ -2154,8 +2154,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="75.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="138"/>
-      <c r="B4" s="149"/>
+      <c r="A4" s="136"/>
+      <c r="B4" s="147"/>
       <c r="C4" s="69" t="s">
         <v>7</v>
       </c>
@@ -2181,11 +2181,11 @@
       <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="138">
+      <c r="A5" s="136">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="141" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="7">
@@ -2217,16 +2217,16 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="146.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="140"/>
-      <c r="B6" s="144"/>
-      <c r="C6" s="121" t="s">
+      <c r="A6" s="138"/>
+      <c r="B6" s="142"/>
+      <c r="C6" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="126" t="s">
+      <c r="D6" s="124" t="s">
         <v>59</v>
       </c>
       <c r="E6" s="57"/>
-      <c r="F6" s="122" t="s">
+      <c r="F6" s="120" t="s">
         <v>60</v>
       </c>
       <c r="G6" s="48"/>
@@ -2236,11 +2236,11 @@
       <c r="I6" s="106"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="141">
+      <c r="A7" s="139">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="145" t="s">
+      <c r="B7" s="143" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="38">
@@ -2273,8 +2273,8 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="142"/>
-      <c r="B8" s="146"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="144"/>
       <c r="C8" s="30" t="s">
         <v>45</v>
       </c>
@@ -2289,14 +2289,14 @@
       <c r="H8" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="132"/>
+      <c r="I8" s="130"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="142">
+      <c r="A9" s="140">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="146"/>
+      <c r="B9" s="144"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2325,18 +2325,18 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L9" s="115"/>
-      <c r="M9" s="115"/>
-      <c r="N9" s="115"/>
-      <c r="O9" s="115"/>
-      <c r="P9" s="115"/>
-      <c r="Q9" s="115"/>
-      <c r="R9" s="115"/>
+      <c r="L9" s="113"/>
+      <c r="M9" s="113"/>
+      <c r="N9" s="113"/>
+      <c r="O9" s="113"/>
+      <c r="P9" s="113"/>
+      <c r="Q9" s="113"/>
+      <c r="R9" s="113"/>
     </row>
     <row r="10" spans="1:18" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="142"/>
-      <c r="B10" s="146"/>
-      <c r="C10" s="131" t="s">
+      <c r="A10" s="140"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="129" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="10" t="s">
@@ -2354,19 +2354,19 @@
       </c>
       <c r="I10" s="13"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="115"/>
-      <c r="N10" s="116"/>
-      <c r="O10" s="115"/>
-      <c r="P10" s="116"/>
-      <c r="Q10" s="115"/>
-      <c r="R10" s="116"/>
+      <c r="M10" s="113"/>
+      <c r="N10" s="114"/>
+      <c r="O10" s="113"/>
+      <c r="P10" s="114"/>
+      <c r="Q10" s="113"/>
+      <c r="R10" s="114"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="142">
+      <c r="A11" s="140">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="146"/>
+      <c r="B11" s="144"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2395,46 +2395,46 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="L11" s="115"/>
-      <c r="M11" s="115"/>
-      <c r="N11" s="115"/>
-      <c r="O11" s="115"/>
-      <c r="P11" s="115"/>
-      <c r="Q11" s="115"/>
-      <c r="R11" s="115"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="113"/>
+      <c r="N11" s="113"/>
+      <c r="O11" s="113"/>
+      <c r="P11" s="113"/>
+      <c r="Q11" s="113"/>
+      <c r="R11" s="113"/>
     </row>
     <row r="12" spans="1:18" ht="102.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="142"/>
-      <c r="B12" s="146"/>
+      <c r="A12" s="140"/>
+      <c r="B12" s="144"/>
       <c r="C12" s="30" t="s">
         <v>68</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="130"/>
+      <c r="E12" s="128"/>
       <c r="F12" s="44" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="42"/>
-      <c r="H12" s="156" t="s">
+      <c r="H12" s="154" t="s">
         <v>73</v>
       </c>
       <c r="I12" s="78"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="115"/>
-      <c r="N12" s="115"/>
-      <c r="O12" s="115"/>
-      <c r="P12" s="116"/>
-      <c r="Q12" s="115"/>
-      <c r="R12" s="116"/>
+      <c r="M12" s="113"/>
+      <c r="N12" s="113"/>
+      <c r="O12" s="113"/>
+      <c r="P12" s="114"/>
+      <c r="Q12" s="113"/>
+      <c r="R12" s="114"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="142">
+      <c r="A13" s="140">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="150" t="s">
+      <c r="B13" s="148" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="17">
@@ -2464,25 +2464,25 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L13" s="115"/>
-      <c r="M13" s="115"/>
-      <c r="N13" s="115"/>
-      <c r="O13" s="115"/>
-      <c r="P13" s="115"/>
-      <c r="Q13" s="115"/>
-      <c r="R13" s="117"/>
+      <c r="L13" s="113"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="113"/>
+      <c r="O13" s="113"/>
+      <c r="P13" s="113"/>
+      <c r="Q13" s="113"/>
+      <c r="R13" s="115"/>
     </row>
     <row r="14" spans="1:18" ht="116.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="147"/>
-      <c r="B14" s="151"/>
-      <c r="C14" s="157" t="s">
+      <c r="A14" s="145"/>
+      <c r="B14" s="149"/>
+      <c r="C14" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="128" t="s">
+      <c r="D14" s="126" t="s">
         <v>75</v>
       </c>
       <c r="E14" s="90"/>
-      <c r="F14" s="127" t="s">
+      <c r="F14" s="125" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="89" t="s">
@@ -2494,20 +2494,20 @@
       <c r="I14" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="117"/>
+      <c r="L14" s="115"/>
       <c r="M14" s="25"/>
-      <c r="N14" s="118"/>
-      <c r="O14" s="115"/>
-      <c r="P14" s="117"/>
-      <c r="Q14" s="115"/>
-      <c r="R14" s="117"/>
+      <c r="N14" s="116"/>
+      <c r="O14" s="113"/>
+      <c r="P14" s="115"/>
+      <c r="Q14" s="113"/>
+      <c r="R14" s="115"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="139">
+      <c r="A15" s="137">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="143" t="s">
+      <c r="B15" s="141" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="67">
@@ -2540,8 +2540,8 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="103.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="140"/>
-      <c r="B16" s="144"/>
+      <c r="A16" s="138"/>
+      <c r="B16" s="142"/>
       <c r="C16" s="86" t="s">
         <v>35</v>
       </c>
@@ -2594,7 +2594,7 @@
       <c r="F18" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="125" t="s">
+      <c r="G18" s="123" t="s">
         <v>56</v>
       </c>
       <c r="H18" s="33" t="s">
@@ -2604,31 +2604,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="120" customFormat="1" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="119"/>
+    <row r="19" spans="1:18" s="118" customFormat="1" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="117"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="117"/>
-      <c r="I19" s="117"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="115"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="115"/>
+      <c r="H19" s="115"/>
+      <c r="I19" s="115"/>
     </row>
     <row r="20" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="134" t="str">
+      <c r="A20" s="132" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
 (as of 2-18-2024, subject to change)</v>
       </c>
-      <c r="B20" s="135"/>
-      <c r="C20" s="135"/>
-      <c r="D20" s="135"/>
-      <c r="E20" s="135"/>
-      <c r="F20" s="135"/>
-      <c r="G20" s="135"/>
-      <c r="H20" s="135"/>
-      <c r="I20" s="136"/>
+      <c r="B20" s="133"/>
+      <c r="C20" s="133"/>
+      <c r="D20" s="133"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="133"/>
+      <c r="G20" s="133"/>
+      <c r="H20" s="133"/>
+      <c r="I20" s="134"/>
     </row>
     <row r="21" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="str">
@@ -2666,11 +2666,11 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="137">
+      <c r="A22" s="135">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B22" s="143" t="s">
+      <c r="B22" s="141" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="95">
@@ -2701,17 +2701,17 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="L22" s="117"/>
-      <c r="M22" s="115"/>
-      <c r="N22" s="115"/>
-      <c r="O22" s="115"/>
-      <c r="P22" s="115"/>
-      <c r="Q22" s="115"/>
-      <c r="R22" s="115"/>
+      <c r="L22" s="115"/>
+      <c r="M22" s="113"/>
+      <c r="N22" s="113"/>
+      <c r="O22" s="113"/>
+      <c r="P22" s="113"/>
+      <c r="Q22" s="113"/>
+      <c r="R22" s="113"/>
     </row>
     <row r="23" spans="1:18" ht="76.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="138"/>
-      <c r="B23" s="143"/>
+      <c r="A23" s="136"/>
+      <c r="B23" s="141"/>
       <c r="C23" s="51"/>
       <c r="D23" s="6" t="s">
         <v>67</v>
@@ -2727,20 +2727,20 @@
         <v>15</v>
       </c>
       <c r="I23" s="35"/>
-      <c r="L23" s="115"/>
-      <c r="M23" s="115"/>
-      <c r="N23" s="115"/>
-      <c r="O23" s="115"/>
-      <c r="P23" s="115"/>
-      <c r="Q23" s="115"/>
+      <c r="L23" s="113"/>
+      <c r="M23" s="113"/>
+      <c r="N23" s="113"/>
+      <c r="O23" s="113"/>
+      <c r="P23" s="113"/>
+      <c r="Q23" s="113"/>
       <c r="R23" s="25"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="138">
+      <c r="A24" s="136">
         <f>A22 - 1</f>
         <v>7</v>
       </c>
-      <c r="B24" s="143"/>
+      <c r="B24" s="141"/>
       <c r="C24" s="7">
         <f>I22 + 1</f>
         <v>17</v>
@@ -2769,22 +2769,22 @@
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="L24" s="115"/>
-      <c r="M24" s="115"/>
-      <c r="N24" s="115"/>
-      <c r="O24" s="115"/>
-      <c r="P24" s="115"/>
-      <c r="Q24" s="115"/>
-      <c r="R24" s="115"/>
+      <c r="L24" s="113"/>
+      <c r="M24" s="113"/>
+      <c r="N24" s="113"/>
+      <c r="O24" s="113"/>
+      <c r="P24" s="113"/>
+      <c r="Q24" s="113"/>
+      <c r="R24" s="113"/>
     </row>
     <row r="25" spans="1:18" ht="124.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="138"/>
-      <c r="B25" s="143"/>
-      <c r="C25" s="114"/>
+      <c r="A25" s="136"/>
+      <c r="B25" s="141"/>
+      <c r="C25" s="112"/>
       <c r="D25" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="133"/>
+      <c r="E25" s="131"/>
       <c r="F25" s="55" t="s">
         <v>43</v>
       </c>
@@ -2794,23 +2794,21 @@
       <c r="H25" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="113" t="s">
-        <v>42</v>
-      </c>
+      <c r="I25" s="157"/>
       <c r="L25" s="25"/>
-      <c r="M25" s="115"/>
-      <c r="N25" s="117"/>
-      <c r="O25" s="115"/>
-      <c r="P25" s="117"/>
-      <c r="Q25" s="115"/>
+      <c r="M25" s="113"/>
+      <c r="N25" s="115"/>
+      <c r="O25" s="113"/>
+      <c r="P25" s="115"/>
+      <c r="Q25" s="113"/>
       <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="138">
+      <c r="A26" s="136">
         <f>A24 - 1</f>
         <v>6</v>
       </c>
-      <c r="B26" s="143"/>
+      <c r="B26" s="141"/>
       <c r="C26" s="7">
         <f>I24 + 1</f>
         <v>24</v>
@@ -2839,18 +2837,20 @@
         <f t="shared" ref="I26" si="9">H26 + 1</f>
         <v>30</v>
       </c>
-      <c r="L26" s="115"/>
-      <c r="M26" s="115"/>
-      <c r="N26" s="115"/>
-      <c r="O26" s="115"/>
-      <c r="P26" s="115"/>
-      <c r="Q26" s="115"/>
-      <c r="R26" s="115"/>
+      <c r="L26" s="113"/>
+      <c r="M26" s="113"/>
+      <c r="N26" s="113"/>
+      <c r="O26" s="113"/>
+      <c r="P26" s="113"/>
+      <c r="Q26" s="113"/>
+      <c r="R26" s="113"/>
     </row>
     <row r="27" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="140"/>
-      <c r="B27" s="144"/>
-      <c r="C27" s="109"/>
+      <c r="A27" s="138"/>
+      <c r="B27" s="142"/>
+      <c r="C27" s="156" t="s">
+        <v>42</v>
+      </c>
       <c r="D27" s="9" t="s">
         <v>22</v>
       </c>
@@ -2858,29 +2858,29 @@
       <c r="F27" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="129" t="s">
+      <c r="G27" s="127" t="s">
         <v>53</v>
       </c>
       <c r="H27" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="I27" s="112" t="s">
+      <c r="I27" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="L27" s="115"/>
-      <c r="M27" s="115"/>
+      <c r="L27" s="113"/>
+      <c r="M27" s="113"/>
       <c r="N27" s="25"/>
-      <c r="O27" s="115"/>
+      <c r="O27" s="113"/>
       <c r="P27" s="25"/>
-      <c r="Q27" s="117"/>
+      <c r="Q27" s="115"/>
       <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="141">
+      <c r="A28" s="139">
         <f>A26 -1</f>
         <v>5</v>
       </c>
-      <c r="B28" s="145" t="s">
+      <c r="B28" s="143" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="101">
@@ -2912,9 +2912,9 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="152"/>
-      <c r="B29" s="151"/>
-      <c r="C29" s="123" t="s">
+      <c r="A29" s="150"/>
+      <c r="B29" s="149"/>
+      <c r="C29" s="121" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="103" t="s">
@@ -2933,11 +2933,11 @@
       <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="153">
+      <c r="A30" s="151">
         <f>A28 -1</f>
         <v>4</v>
       </c>
-      <c r="B30" s="145" t="s">
+      <c r="B30" s="143" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="60">
@@ -2970,13 +2970,13 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="142"/>
-      <c r="B31" s="146"/>
+      <c r="A31" s="140"/>
+      <c r="B31" s="144"/>
       <c r="C31" s="29"/>
-      <c r="D31" s="110" t="s">
+      <c r="D31" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="111" t="s">
+      <c r="E31" s="110" t="s">
         <v>72</v>
       </c>
       <c r="F31" s="12" t="s">
@@ -2989,11 +2989,11 @@
       <c r="I31" s="28"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="142">
+      <c r="A32" s="140">
         <f>A30 -1</f>
         <v>3</v>
       </c>
-      <c r="B32" s="146"/>
+      <c r="B32" s="144"/>
       <c r="C32" s="27">
         <f>I30 + 1</f>
         <v>14</v>
@@ -3024,8 +3024,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="142"/>
-      <c r="B33" s="146"/>
+      <c r="A33" s="140"/>
+      <c r="B33" s="144"/>
       <c r="C33" s="29"/>
       <c r="D33" s="104" t="s">
         <v>6</v>
@@ -3043,11 +3043,11 @@
       <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="142">
+      <c r="A34" s="140">
         <f>A32 -1</f>
         <v>2</v>
       </c>
-      <c r="B34" s="146"/>
+      <c r="B34" s="144"/>
       <c r="C34" s="29">
         <f>I32 + 1</f>
         <v>21</v>
@@ -3078,8 +3078,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="147"/>
-      <c r="B35" s="151"/>
+      <c r="A35" s="145"/>
+      <c r="B35" s="149"/>
       <c r="C35" s="58"/>
       <c r="D35" s="43" t="s">
         <v>23</v>
@@ -3095,11 +3095,11 @@
       <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="139">
+      <c r="A36" s="137">
         <f>A34 -1</f>
         <v>1</v>
       </c>
-      <c r="B36" s="148" t="s">
+      <c r="B36" s="146" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="17">
@@ -3131,8 +3131,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="140"/>
-      <c r="B37" s="144"/>
+      <c r="A37" s="138"/>
+      <c r="B37" s="142"/>
       <c r="C37" s="98"/>
       <c r="D37" s="49" t="s">
         <v>6</v>
@@ -3145,15 +3145,15 @@
       <c r="H37" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I37" s="124" t="s">
+      <c r="I37" s="122" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="154" t="s">
+      <c r="A38" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="143" t="s">
+      <c r="B38" s="141" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="20">
@@ -3186,8 +3186,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="155"/>
-      <c r="B39" s="144"/>
+      <c r="A39" s="153"/>
+      <c r="B39" s="142"/>
       <c r="C39" s="61" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
updated Team MS1 due date
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar.xlsx
+++ b/CS320-Spring2024Calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DDC433-3FE3-4EDE-A9A6-29350849E125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63354E58-BAF0-458D-AD45-D9CBD305D903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1425" windowWidth="25620" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="698" yWindow="593" windowWidth="27307" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp24" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
   <si>
     <t>Monday</t>
   </si>
@@ -498,9 +498,6 @@
 (Marmoset)</t>
   </si>
   <si>
-    <t>(Marmoset)</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A09: Individual  Report 
 due 4-10-24
@@ -576,16 +573,15 @@
     </r>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>Team Session:
-Final Preparation for Milestone 1
+    <t>CS320: SW Engineering - Spring 2024 Schedule
+(as of 3-11-2024, subject to change)</t>
+  </si>
+  <si>
+    <t>Team Session: Final Preparation for Milestone 1
 (in-class)</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2024 Schedule
-(as of 2-28-2024, subject to change)</t>
+    <t>Assign06: Team Problem Domain Analysis Submission Review</t>
   </si>
 </sst>
 </file>
@@ -1688,77 +1684,77 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2069,8 +2065,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2092,17 +2088,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="134" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="136"/>
+      <c r="A1" s="152" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="154"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2132,10 +2128,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="139">
+      <c r="A3" s="144">
         <v>15</v>
       </c>
-      <c r="B3" s="148" t="s">
+      <c r="B3" s="139" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="66">
@@ -2167,8 +2163,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="75.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="138"/>
-      <c r="B4" s="149"/>
+      <c r="A4" s="148"/>
+      <c r="B4" s="156"/>
       <c r="C4" s="68" t="s">
         <v>7</v>
       </c>
@@ -2194,11 +2190,11 @@
       <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="138">
+      <c r="A5" s="148">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="141" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="7">
@@ -2230,8 +2226,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="146.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="140"/>
-      <c r="B6" s="144"/>
+      <c r="A6" s="145"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="117" t="s">
         <v>55</v>
       </c>
@@ -2249,11 +2245,11 @@
       <c r="I6" s="104"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="141">
+      <c r="A7" s="149">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="145" t="s">
+      <c r="B7" s="136" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="38">
@@ -2287,7 +2283,7 @@
     </row>
     <row r="8" spans="1:18" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="142"/>
-      <c r="B8" s="146"/>
+      <c r="B8" s="138"/>
       <c r="C8" s="30" t="s">
         <v>43</v>
       </c>
@@ -2309,7 +2305,7 @@
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="146"/>
+      <c r="B9" s="138"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2348,7 +2344,7 @@
     </row>
     <row r="10" spans="1:18" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="142"/>
-      <c r="B10" s="146"/>
+      <c r="B10" s="138"/>
       <c r="C10" s="126" t="s">
         <v>38</v>
       </c>
@@ -2379,7 +2375,7 @@
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="146"/>
+      <c r="B11" s="138"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2418,22 +2414,22 @@
     </row>
     <row r="12" spans="1:18" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="142"/>
-      <c r="B12" s="146"/>
+      <c r="B12" s="138"/>
       <c r="C12" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="133" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G12" s="42"/>
       <c r="H12" s="129" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I12" s="77"/>
       <c r="L12" s="25"/>
@@ -2449,7 +2445,7 @@
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="150" t="s">
+      <c r="B13" s="157" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="17">
@@ -2488,13 +2484,13 @@
       <c r="R13" s="113"/>
     </row>
     <row r="14" spans="1:18" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="147"/>
-      <c r="B14" s="151"/>
+      <c r="A14" s="143"/>
+      <c r="B14" s="137"/>
       <c r="C14" s="130" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="124" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="89"/>
       <c r="F14" s="123" t="s">
@@ -2518,11 +2514,11 @@
       <c r="R14" s="113"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="139">
+      <c r="A15" s="144">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="143" t="s">
+      <c r="B15" s="141" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="66">
@@ -2555,8 +2551,8 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="103.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="140"/>
-      <c r="B16" s="144"/>
+      <c r="A16" s="145"/>
+      <c r="B16" s="140"/>
       <c r="C16" s="85" t="s">
         <v>33</v>
       </c>
@@ -2583,8 +2579,8 @@
 Team MS1 Prep
 (all in-class)</v>
       </c>
-      <c r="I16" s="156" t="s">
-        <v>70</v>
+      <c r="I16" s="134" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="6.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2633,19 +2629,19 @@
       <c r="I19" s="113"/>
     </row>
     <row r="20" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="134" t="str">
+      <c r="A20" s="152" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
-(as of 2-28-2024, subject to change)</v>
-      </c>
-      <c r="B20" s="135"/>
-      <c r="C20" s="135"/>
-      <c r="D20" s="135"/>
-      <c r="E20" s="135"/>
-      <c r="F20" s="135"/>
-      <c r="G20" s="135"/>
-      <c r="H20" s="135"/>
-      <c r="I20" s="136"/>
+(as of 3-11-2024, subject to change)</v>
+      </c>
+      <c r="B20" s="153"/>
+      <c r="C20" s="153"/>
+      <c r="D20" s="153"/>
+      <c r="E20" s="153"/>
+      <c r="F20" s="153"/>
+      <c r="G20" s="153"/>
+      <c r="H20" s="153"/>
+      <c r="I20" s="154"/>
     </row>
     <row r="21" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="str">
@@ -2683,11 +2679,11 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="137">
+      <c r="A22" s="155">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B22" s="143" t="s">
+      <c r="B22" s="141" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="93">
@@ -2726,20 +2722,20 @@
       <c r="Q22" s="111"/>
       <c r="R22" s="111"/>
     </row>
-    <row r="23" spans="1:18" ht="76.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="138"/>
-      <c r="B23" s="143"/>
-      <c r="C23" s="157"/>
+    <row r="23" spans="1:18" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="148"/>
+      <c r="B23" s="141"/>
+      <c r="C23" s="135"/>
       <c r="D23" s="6" t="s">
         <v>77</v>
       </c>
       <c r="E23" s="54"/>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="22" t="s">
         <v>14</v>
-      </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="I23" s="35"/>
       <c r="L23" s="111"/>
@@ -2751,11 +2747,11 @@
       <c r="R23" s="25"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="138">
+      <c r="A24" s="148">
         <f>A22 - 1</f>
         <v>7</v>
       </c>
-      <c r="B24" s="143"/>
+      <c r="B24" s="141"/>
       <c r="C24" s="7">
         <f>I22 + 1</f>
         <v>17</v>
@@ -2793,8 +2789,8 @@
       <c r="R24" s="111"/>
     </row>
     <row r="25" spans="1:18" ht="124.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="138"/>
-      <c r="B25" s="143"/>
+      <c r="A25" s="148"/>
+      <c r="B25" s="141"/>
       <c r="C25" s="110"/>
       <c r="D25" s="26" t="s">
         <v>24</v>
@@ -2819,11 +2815,11 @@
       <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="138">
+      <c r="A26" s="148">
         <f>A24 - 1</f>
         <v>6</v>
       </c>
-      <c r="B26" s="143"/>
+      <c r="B26" s="141"/>
       <c r="C26" s="7">
         <f>I24 + 1</f>
         <v>24</v>
@@ -2861,8 +2857,8 @@
       <c r="R26" s="111"/>
     </row>
     <row r="27" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="140"/>
-      <c r="B27" s="144"/>
+      <c r="A27" s="145"/>
+      <c r="B27" s="140"/>
       <c r="C27" s="131" t="s">
         <v>40</v>
       </c>
@@ -2891,11 +2887,11 @@
       <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="141">
+      <c r="A28" s="149">
         <f>A26 -1</f>
         <v>5</v>
       </c>
-      <c r="B28" s="145" t="s">
+      <c r="B28" s="136" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="99">
@@ -2927,8 +2923,8 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="152"/>
-      <c r="B29" s="151"/>
+      <c r="A29" s="150"/>
+      <c r="B29" s="137"/>
       <c r="C29" s="119" t="s">
         <v>37</v>
       </c>
@@ -2948,11 +2944,11 @@
       <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="153">
+      <c r="A30" s="151">
         <f>A28 -1</f>
         <v>4</v>
       </c>
-      <c r="B30" s="145" t="s">
+      <c r="B30" s="136" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="59">
@@ -2986,13 +2982,13 @@
     </row>
     <row r="31" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="142"/>
-      <c r="B31" s="146"/>
+      <c r="B31" s="138"/>
       <c r="C31" s="29"/>
       <c r="D31" s="107" t="s">
         <v>25</v>
       </c>
       <c r="E31" s="108" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>45</v>
@@ -3008,7 +3004,7 @@
         <f>A30 -1</f>
         <v>3</v>
       </c>
-      <c r="B32" s="146"/>
+      <c r="B32" s="138"/>
       <c r="C32" s="27">
         <f>I30 + 1</f>
         <v>14</v>
@@ -3040,14 +3036,12 @@
     </row>
     <row r="33" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="142"/>
-      <c r="B33" s="146"/>
+      <c r="B33" s="138"/>
       <c r="C33" s="29"/>
       <c r="D33" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="11" t="s">
-        <v>67</v>
-      </c>
+      <c r="E33" s="11"/>
       <c r="F33" s="44" t="s">
         <v>6</v>
       </c>
@@ -3062,7 +3056,7 @@
         <f>A32 -1</f>
         <v>2</v>
       </c>
-      <c r="B34" s="146"/>
+      <c r="B34" s="138"/>
       <c r="C34" s="29">
         <f>I32 + 1</f>
         <v>21</v>
@@ -3093,8 +3087,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="147"/>
-      <c r="B35" s="151"/>
+      <c r="A35" s="143"/>
+      <c r="B35" s="137"/>
       <c r="C35" s="57"/>
       <c r="D35" s="43" t="s">
         <v>22</v>
@@ -3110,11 +3104,11 @@
       <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="139">
+      <c r="A36" s="144">
         <f>A34 -1</f>
         <v>1</v>
       </c>
-      <c r="B36" s="148" t="s">
+      <c r="B36" s="139" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="17">
@@ -3146,8 +3140,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="140"/>
-      <c r="B37" s="144"/>
+      <c r="A37" s="145"/>
+      <c r="B37" s="140"/>
       <c r="C37" s="96"/>
       <c r="D37" s="49" t="s">
         <v>6</v>
@@ -3165,10 +3159,10 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="154" t="s">
+      <c r="A38" s="146" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="143" t="s">
+      <c r="B38" s="141" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="20">
@@ -3201,8 +3195,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="155"/>
-      <c r="B39" s="144"/>
+      <c r="A39" s="147"/>
+      <c r="B39" s="140"/>
       <c r="C39" s="60" t="s">
         <v>42</v>
       </c>
@@ -3220,18 +3214,6 @@
     <row r="40" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A3:A4"/>
@@ -3248,6 +3230,18 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>

</xml_diff>

<commit_message>
updated lab due dates
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar.xlsx
+++ b/CS320-Spring2024Calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63354E58-BAF0-458D-AD45-D9CBD305D903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4166887-8506-437A-B465-9E33C6DF1E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="698" yWindow="593" windowWidth="27307" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="26264" windowHeight="15127" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp24" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Monday</t>
   </si>
@@ -95,10 +95,6 @@
   </si>
   <si>
     <t>Legend</t>
-  </si>
-  <si>
-    <t>A03: Team MS2
-50% Progress on Features</t>
   </si>
   <si>
     <t>SQL/JDBC/ORM Review &amp; Labs
@@ -164,16 +160,6 @@
   </si>
   <si>
     <t>A02: Individual Project Proposal due Noon
-(Marmoset)</t>
-  </si>
-  <si>
-    <t>Lab 4: SQL
-due Noon
-(Marmoset)</t>
-  </si>
-  <si>
-    <t>Lab 5: JDBC
-due Noon
 (Marmoset)</t>
   </si>
   <si>
@@ -277,24 +263,6 @@
 Peer Evals
 due Noon
 (Marmoset)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lecture  15: ORM, Designing a Persistence Layer
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 6: ORM
-(assigned)</t>
-    </r>
   </si>
   <si>
     <t>Individual Lab or Assignment Due</t>
@@ -573,15 +541,47 @@
     </r>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2024 Schedule
-(as of 3-11-2024, subject to change)</t>
-  </si>
-  <si>
     <t>Team Session: Final Preparation for Milestone 1
 (in-class)</t>
   </si>
   <si>
     <t>Assign06: Team Problem Domain Analysis Submission Review</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2024 Schedule
+(as of 3-19-2024, subject to change)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lecture  15: ORM, Designing a Persistence Layer
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 6: ORM
+(assigned)
+Lab 4: SQL
+due by 10:00a
+(Marmoset)</t>
+    </r>
+  </si>
+  <si>
+    <t>Lab 5: JDBC
+due 10:00a
+Mon, 3-25-24
+-------------&gt;&gt;&gt;&gt;
+(Marmoset)</t>
+  </si>
+  <si>
+    <t>A03: Team MS2
+50% Progress on Features w/fake data</t>
   </si>
 </sst>
 </file>
@@ -1600,9 +1600,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1689,35 +1686,65 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1726,35 +1753,8 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2065,8 +2065,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2088,17 +2088,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="152" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
-      <c r="G1" s="153"/>
-      <c r="H1" s="153"/>
-      <c r="I1" s="154"/>
+      <c r="A1" s="135" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="137"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2128,10 +2128,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="144">
+      <c r="A3" s="140">
         <v>15</v>
       </c>
-      <c r="B3" s="139" t="s">
+      <c r="B3" s="149" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="66">
@@ -2163,8 +2163,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="75.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="148"/>
-      <c r="B4" s="156"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="150"/>
       <c r="C4" s="68" t="s">
         <v>7</v>
       </c>
@@ -2185,17 +2185,17 @@
       </c>
       <c r="G4" s="37"/>
       <c r="H4" s="36" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="148">
+      <c r="A5" s="139">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="141" t="s">
-        <v>28</v>
+      <c r="B5" s="144" t="s">
+        <v>27</v>
       </c>
       <c r="C5" s="7">
         <f>I3 + 1</f>
@@ -2226,30 +2226,30 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="146.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="145"/>
-      <c r="B6" s="140"/>
-      <c r="C6" s="117" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="122" t="s">
-        <v>57</v>
+      <c r="A6" s="141"/>
+      <c r="B6" s="145"/>
+      <c r="C6" s="116" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="121" t="s">
+        <v>53</v>
       </c>
       <c r="E6" s="56"/>
-      <c r="F6" s="118" t="s">
-        <v>58</v>
+      <c r="F6" s="117" t="s">
+        <v>54</v>
       </c>
       <c r="G6" s="48"/>
       <c r="H6" s="47" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I6" s="104"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="149">
+      <c r="A7" s="142">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="136" t="s">
+      <c r="B7" s="146" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="38">
@@ -2282,30 +2282,30 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="142"/>
-      <c r="B8" s="138"/>
+      <c r="A8" s="143"/>
+      <c r="B8" s="147"/>
       <c r="C8" s="30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G8" s="27"/>
       <c r="H8" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8" s="127"/>
+        <v>61</v>
+      </c>
+      <c r="I8" s="126"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="142">
+      <c r="A9" s="143">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="138"/>
+      <c r="B9" s="147"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2334,48 +2334,48 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L9" s="111"/>
-      <c r="M9" s="111"/>
-      <c r="N9" s="111"/>
-      <c r="O9" s="111"/>
-      <c r="P9" s="111"/>
-      <c r="Q9" s="111"/>
-      <c r="R9" s="111"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="110"/>
+      <c r="N9" s="110"/>
+      <c r="O9" s="110"/>
+      <c r="P9" s="110"/>
+      <c r="Q9" s="110"/>
+      <c r="R9" s="110"/>
     </row>
     <row r="10" spans="1:18" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="142"/>
-      <c r="B10" s="138"/>
-      <c r="C10" s="126" t="s">
-        <v>38</v>
+      <c r="A10" s="143"/>
+      <c r="B10" s="147"/>
+      <c r="C10" s="125" t="s">
+        <v>37</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="105" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I10" s="13"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="111"/>
-      <c r="N10" s="112"/>
-      <c r="O10" s="111"/>
-      <c r="P10" s="112"/>
-      <c r="Q10" s="111"/>
-      <c r="R10" s="112"/>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
+      <c r="O10" s="110"/>
+      <c r="P10" s="111"/>
+      <c r="Q10" s="110"/>
+      <c r="R10" s="111"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="142">
+      <c r="A11" s="143">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="138"/>
+      <c r="B11" s="147"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2404,49 +2404,49 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="L11" s="111"/>
-      <c r="M11" s="111"/>
-      <c r="N11" s="111"/>
-      <c r="O11" s="111"/>
-      <c r="P11" s="111"/>
-      <c r="Q11" s="111"/>
-      <c r="R11" s="111"/>
+      <c r="L11" s="110"/>
+      <c r="M11" s="110"/>
+      <c r="N11" s="110"/>
+      <c r="O11" s="110"/>
+      <c r="P11" s="110"/>
+      <c r="Q11" s="110"/>
+      <c r="R11" s="110"/>
     </row>
     <row r="12" spans="1:18" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="142"/>
-      <c r="B12" s="138"/>
+      <c r="A12" s="143"/>
+      <c r="B12" s="147"/>
       <c r="C12" s="30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="133" t="s">
-        <v>70</v>
+        <v>31</v>
+      </c>
+      <c r="E12" s="132" t="s">
+        <v>66</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G12" s="42"/>
-      <c r="H12" s="129" t="s">
-        <v>72</v>
+      <c r="H12" s="128" t="s">
+        <v>68</v>
       </c>
       <c r="I12" s="77"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="111"/>
-      <c r="N12" s="111"/>
-      <c r="O12" s="111"/>
-      <c r="P12" s="112"/>
-      <c r="Q12" s="111"/>
-      <c r="R12" s="112"/>
+      <c r="M12" s="110"/>
+      <c r="N12" s="110"/>
+      <c r="O12" s="110"/>
+      <c r="P12" s="111"/>
+      <c r="Q12" s="110"/>
+      <c r="R12" s="111"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="142">
+      <c r="A13" s="143">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="157" t="s">
-        <v>29</v>
+      <c r="B13" s="151" t="s">
+        <v>28</v>
       </c>
       <c r="C13" s="17">
         <f>I11 + 1</f>
@@ -2475,50 +2475,50 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L13" s="111"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="111"/>
-      <c r="O13" s="111"/>
-      <c r="P13" s="111"/>
-      <c r="Q13" s="111"/>
-      <c r="R13" s="113"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="110"/>
+      <c r="N13" s="110"/>
+      <c r="O13" s="110"/>
+      <c r="P13" s="110"/>
+      <c r="Q13" s="110"/>
+      <c r="R13" s="112"/>
     </row>
     <row r="14" spans="1:18" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="143"/>
-      <c r="B14" s="137"/>
-      <c r="C14" s="130" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="124" t="s">
-        <v>74</v>
+      <c r="A14" s="148"/>
+      <c r="B14" s="152"/>
+      <c r="C14" s="129" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="123" t="s">
+        <v>70</v>
       </c>
       <c r="E14" s="89"/>
-      <c r="F14" s="123" t="s">
-        <v>23</v>
+      <c r="F14" s="122" t="s">
+        <v>22</v>
       </c>
       <c r="G14" s="88" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="83" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I14" s="84" t="s">
-        <v>33</v>
-      </c>
-      <c r="L14" s="113"/>
+        <v>32</v>
+      </c>
+      <c r="L14" s="112"/>
       <c r="M14" s="25"/>
-      <c r="N14" s="114"/>
-      <c r="O14" s="111"/>
-      <c r="P14" s="113"/>
-      <c r="Q14" s="111"/>
-      <c r="R14" s="113"/>
+      <c r="N14" s="113"/>
+      <c r="O14" s="110"/>
+      <c r="P14" s="112"/>
+      <c r="Q14" s="110"/>
+      <c r="R14" s="112"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="144">
+      <c r="A15" s="140">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="141" t="s">
+      <c r="B15" s="144" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="66">
@@ -2551,16 +2551,16 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="103.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="145"/>
-      <c r="B16" s="140"/>
+      <c r="A16" s="141"/>
+      <c r="B16" s="145"/>
       <c r="C16" s="85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E16" s="63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" s="9" t="str">
         <f>D16</f>
@@ -2579,8 +2579,8 @@
 Team MS1 Prep
 (all in-class)</v>
       </c>
-      <c r="I16" s="134" t="s">
-        <v>69</v>
+      <c r="I16" s="133" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="6.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2602,46 +2602,46 @@
         <v>15</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F18" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="121" t="s">
-        <v>54</v>
+      <c r="G18" s="120" t="s">
+        <v>50</v>
       </c>
       <c r="H18" s="33" t="s">
         <v>17</v>
       </c>
       <c r="I18" s="62" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" s="116" customFormat="1" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="115"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="115" customFormat="1" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="114"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
-      <c r="G19" s="113"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="113"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
     </row>
     <row r="20" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="152" t="str">
+      <c r="A20" s="135" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
-(as of 3-11-2024, subject to change)</v>
-      </c>
-      <c r="B20" s="153"/>
-      <c r="C20" s="153"/>
-      <c r="D20" s="153"/>
-      <c r="E20" s="153"/>
-      <c r="F20" s="153"/>
-      <c r="G20" s="153"/>
-      <c r="H20" s="153"/>
-      <c r="I20" s="154"/>
+(as of 3-19-2024, subject to change)</v>
+      </c>
+      <c r="B20" s="136"/>
+      <c r="C20" s="136"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="136"/>
+      <c r="G20" s="136"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="137"/>
     </row>
     <row r="21" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="str">
@@ -2679,11 +2679,11 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="155">
+      <c r="A22" s="138">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B22" s="141" t="s">
+      <c r="B22" s="144" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="93">
@@ -2714,44 +2714,44 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="L22" s="113"/>
-      <c r="M22" s="111"/>
-      <c r="N22" s="111"/>
-      <c r="O22" s="111"/>
-      <c r="P22" s="111"/>
-      <c r="Q22" s="111"/>
-      <c r="R22" s="111"/>
+      <c r="L22" s="112"/>
+      <c r="M22" s="110"/>
+      <c r="N22" s="110"/>
+      <c r="O22" s="110"/>
+      <c r="P22" s="110"/>
+      <c r="Q22" s="110"/>
+      <c r="R22" s="110"/>
     </row>
     <row r="23" spans="1:18" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="148"/>
-      <c r="B23" s="141"/>
-      <c r="C23" s="135"/>
+      <c r="A23" s="139"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="134"/>
       <c r="D23" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E23" s="54"/>
       <c r="F23" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="22" t="s">
         <v>14</v>
       </c>
       <c r="I23" s="35"/>
-      <c r="L23" s="111"/>
-      <c r="M23" s="111"/>
-      <c r="N23" s="111"/>
-      <c r="O23" s="111"/>
-      <c r="P23" s="111"/>
-      <c r="Q23" s="111"/>
+      <c r="L23" s="110"/>
+      <c r="M23" s="110"/>
+      <c r="N23" s="110"/>
+      <c r="O23" s="110"/>
+      <c r="P23" s="110"/>
+      <c r="Q23" s="110"/>
       <c r="R23" s="25"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="148">
+      <c r="A24" s="139">
         <f>A22 - 1</f>
         <v>7</v>
       </c>
-      <c r="B24" s="141"/>
+      <c r="B24" s="144"/>
       <c r="C24" s="7">
         <f>I22 + 1</f>
         <v>17</v>
@@ -2780,46 +2780,44 @@
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="L24" s="111"/>
-      <c r="M24" s="111"/>
-      <c r="N24" s="111"/>
-      <c r="O24" s="111"/>
-      <c r="P24" s="111"/>
-      <c r="Q24" s="111"/>
-      <c r="R24" s="111"/>
+      <c r="L24" s="110"/>
+      <c r="M24" s="110"/>
+      <c r="N24" s="110"/>
+      <c r="O24" s="110"/>
+      <c r="P24" s="110"/>
+      <c r="Q24" s="110"/>
+      <c r="R24" s="110"/>
     </row>
     <row r="25" spans="1:18" ht="124.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="148"/>
-      <c r="B25" s="141"/>
-      <c r="C25" s="110"/>
+      <c r="A25" s="139"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="109"/>
       <c r="D25" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="128"/>
+        <v>23</v>
+      </c>
+      <c r="E25" s="127"/>
       <c r="F25" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="106" t="s">
-        <v>39</v>
-      </c>
-      <c r="H25" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="I25" s="132"/>
+        <v>38</v>
+      </c>
+      <c r="G25" s="127"/>
+      <c r="H25" s="157" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" s="131"/>
       <c r="L25" s="25"/>
-      <c r="M25" s="111"/>
-      <c r="N25" s="113"/>
-      <c r="O25" s="111"/>
-      <c r="P25" s="113"/>
-      <c r="Q25" s="111"/>
+      <c r="M25" s="110"/>
+      <c r="N25" s="112"/>
+      <c r="O25" s="110"/>
+      <c r="P25" s="112"/>
+      <c r="Q25" s="110"/>
       <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="148">
+      <c r="A26" s="139">
         <f>A24 - 1</f>
         <v>6</v>
       </c>
-      <c r="B26" s="141"/>
+      <c r="B26" s="144"/>
       <c r="C26" s="7">
         <f>I24 + 1</f>
         <v>24</v>
@@ -2848,51 +2846,51 @@
         <f t="shared" ref="I26" si="9">H26 + 1</f>
         <v>30</v>
       </c>
-      <c r="L26" s="111"/>
-      <c r="M26" s="111"/>
-      <c r="N26" s="111"/>
-      <c r="O26" s="111"/>
-      <c r="P26" s="111"/>
-      <c r="Q26" s="111"/>
-      <c r="R26" s="111"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="110"/>
+      <c r="N26" s="110"/>
+      <c r="O26" s="110"/>
+      <c r="P26" s="110"/>
+      <c r="Q26" s="110"/>
+      <c r="R26" s="110"/>
     </row>
     <row r="27" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="145"/>
-      <c r="B27" s="140"/>
-      <c r="C27" s="131" t="s">
-        <v>40</v>
+      <c r="A27" s="141"/>
+      <c r="B27" s="145"/>
+      <c r="C27" s="130" t="s">
+        <v>75</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E27" s="54"/>
       <c r="F27" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="125" t="s">
-        <v>51</v>
+        <v>76</v>
+      </c>
+      <c r="G27" s="124" t="s">
+        <v>48</v>
       </c>
       <c r="H27" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="I27" s="109" t="s">
-        <v>37</v>
-      </c>
-      <c r="L27" s="111"/>
-      <c r="M27" s="111"/>
+        <v>36</v>
+      </c>
+      <c r="I27" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" s="110"/>
+      <c r="M27" s="110"/>
       <c r="N27" s="25"/>
-      <c r="O27" s="111"/>
+      <c r="O27" s="110"/>
       <c r="P27" s="25"/>
-      <c r="Q27" s="113"/>
+      <c r="Q27" s="112"/>
       <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="149">
+      <c r="A28" s="142">
         <f>A26 -1</f>
         <v>5</v>
       </c>
-      <c r="B28" s="136" t="s">
-        <v>34</v>
+      <c r="B28" s="146" t="s">
+        <v>33</v>
       </c>
       <c r="C28" s="99">
         <f>I26 + 1</f>
@@ -2923,32 +2921,32 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="150"/>
-      <c r="B29" s="137"/>
-      <c r="C29" s="119" t="s">
-        <v>37</v>
+      <c r="A29" s="153"/>
+      <c r="B29" s="152"/>
+      <c r="C29" s="118" t="s">
+        <v>36</v>
       </c>
       <c r="D29" s="101" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G29" s="78"/>
       <c r="H29" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="151">
+      <c r="A30" s="154">
         <f>A28 -1</f>
         <v>4</v>
       </c>
-      <c r="B30" s="136" t="s">
+      <c r="B30" s="146" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="59">
@@ -2981,30 +2979,30 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="142"/>
-      <c r="B31" s="138"/>
+      <c r="A31" s="143"/>
+      <c r="B31" s="147"/>
       <c r="C31" s="29"/>
-      <c r="D31" s="107" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="108" t="s">
-        <v>67</v>
+      <c r="D31" s="106" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="107" t="s">
+        <v>63</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G31" s="27"/>
       <c r="H31" s="103" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I31" s="28"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="142">
+      <c r="A32" s="143">
         <f>A30 -1</f>
         <v>3</v>
       </c>
-      <c r="B32" s="138"/>
+      <c r="B32" s="147"/>
       <c r="C32" s="27">
         <f>I30 + 1</f>
         <v>14</v>
@@ -3035,8 +3033,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="142"/>
-      <c r="B33" s="138"/>
+      <c r="A33" s="143"/>
+      <c r="B33" s="147"/>
       <c r="C33" s="29"/>
       <c r="D33" s="102" t="s">
         <v>6</v>
@@ -3052,11 +3050,11 @@
       <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="142">
+      <c r="A34" s="143">
         <f>A32 -1</f>
         <v>2</v>
       </c>
-      <c r="B34" s="138"/>
+      <c r="B34" s="147"/>
       <c r="C34" s="29">
         <f>I32 + 1</f>
         <v>21</v>
@@ -3087,11 +3085,11 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="143"/>
-      <c r="B35" s="137"/>
+      <c r="A35" s="148"/>
+      <c r="B35" s="152"/>
       <c r="C35" s="57"/>
       <c r="D35" s="43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35" s="42"/>
       <c r="F35" s="44" t="s">
@@ -3104,12 +3102,12 @@
       <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="144">
+      <c r="A36" s="140">
         <f>A34 -1</f>
         <v>1</v>
       </c>
-      <c r="B36" s="139" t="s">
-        <v>35</v>
+      <c r="B36" s="149" t="s">
+        <v>34</v>
       </c>
       <c r="C36" s="17">
         <f>I34 + 1</f>
@@ -3140,8 +3138,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="145"/>
-      <c r="B37" s="140"/>
+      <c r="A37" s="141"/>
+      <c r="B37" s="145"/>
       <c r="C37" s="96"/>
       <c r="D37" s="49" t="s">
         <v>6</v>
@@ -3152,17 +3150,17 @@
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I37" s="120" t="s">
-        <v>49</v>
+        <v>30</v>
+      </c>
+      <c r="I37" s="119" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="146" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="141" t="s">
+      <c r="A38" s="155" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="144" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="20">
@@ -3195,17 +3193,17 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="147"/>
-      <c r="B39" s="140"/>
+      <c r="A39" s="156"/>
+      <c r="B39" s="145"/>
       <c r="C39" s="60" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E39" s="61"/>
       <c r="F39" s="23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G39" s="21"/>
       <c r="H39" s="75"/>
@@ -3214,6 +3212,18 @@
     <row r="40" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A3:A4"/>
@@ -3230,18 +3240,6 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>

</xml_diff>